<commit_message>
WAT new API's automation
</commit_message>
<xml_diff>
--- a/src/test/test-data/WATTestData.xlsx
+++ b/src/test/test-data/WATTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="139">
   <si>
     <t>GET</t>
   </si>
@@ -407,6 +407,57 @@
   </si>
   <si>
     <t>WAT-387</t>
+  </si>
+  <si>
+    <t>Verify that user is able to search for author cluster using ORCID</t>
+  </si>
+  <si>
+    <t>Verify that user is able to search for author cluster using RID</t>
+  </si>
+  <si>
+    <t>recommend/search/author/clusters/</t>
+  </si>
+  <si>
+    <t>recommend/search/author/clusters/0000-0002-6423-7213</t>
+  </si>
+  <si>
+    <t>Verify that user is able to search author cluster when ORCID/RID is missing in the request</t>
+  </si>
+  <si>
+    <t>recommend/search/author/clusters/A-9832-2009</t>
+  </si>
+  <si>
+    <t>recommend/search/author/clusters/0000-abcd-6423-12ec</t>
+  </si>
+  <si>
+    <t>status=200||hits.authorClusterId=24303705</t>
+  </si>
+  <si>
+    <t>status=200||hits.authorClusterId=80453160</t>
+  </si>
+  <si>
+    <t>Verify that user is able to search author cluster using invalid ORCID</t>
+  </si>
+  <si>
+    <t>Verify that user is able to search author cluster using invalid RID</t>
+  </si>
+  <si>
+    <t>WAT-408</t>
+  </si>
+  <si>
+    <t>WAT-409</t>
+  </si>
+  <si>
+    <t>WAT-504</t>
+  </si>
+  <si>
+    <t>WAT-505</t>
+  </si>
+  <si>
+    <t>WAT-506</t>
+  </si>
+  <si>
+    <t>recommend/search/author/clusters/A-1456-abcs</t>
   </si>
 </sst>
 </file>
@@ -854,10 +905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1714,19 +1765,153 @@
       <c r="E28" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F28" s="10"/>
-      <c r="G28" s="8" t="s">
+      <c r="F28" s="15"/>
+      <c r="G28" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="7" t="s">
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="K28" s="9"/>
+      <c r="K28" s="16"/>
       <c r="L28" t="s">
         <v>114</v>
       </c>
+    </row>
+    <row r="29" spans="1:12" ht="120">
+      <c r="A29" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F29" s="10"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="L29" s="9"/>
+    </row>
+    <row r="30" spans="1:12" ht="120">
+      <c r="A30" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F30" s="10"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="L30" s="9"/>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F31" s="10"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F32" s="10"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F33" s="10"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
WAT API test scripts
</commit_message>
<xml_diff>
--- a/src/test/test-data/WATTestData.xlsx
+++ b/src/test/test-data/WATTestData.xlsx
@@ -415,21 +415,9 @@
     <t>Verify that user is able to search for author cluster using RID</t>
   </si>
   <si>
-    <t>recommend/search/author/clusters/</t>
-  </si>
-  <si>
-    <t>recommend/search/author/clusters/0000-0002-6423-7213</t>
-  </si>
-  <si>
     <t>Verify that user is able to search author cluster when ORCID/RID is missing in the request</t>
   </si>
   <si>
-    <t>recommend/search/author/clusters/A-9832-2009</t>
-  </si>
-  <si>
-    <t>recommend/search/author/clusters/0000-abcd-6423-12ec</t>
-  </si>
-  <si>
     <t>status=200||hits.authorClusterId=24303705</t>
   </si>
   <si>
@@ -457,7 +445,19 @@
     <t>WAT-506</t>
   </si>
   <si>
-    <t>recommend/search/author/clusters/A-1456-abcs</t>
+    <t>/recommend/search/author/clusters/0000-0002-6423-7213</t>
+  </si>
+  <si>
+    <t>/recommend/search/author/clusters/A-9832-2009</t>
+  </si>
+  <si>
+    <t>/recommend/search/author/clusters/</t>
+  </si>
+  <si>
+    <t>/recommend/search/author/clusters/0000-abcd-6423-12ec</t>
+  </si>
+  <si>
+    <t>/recommend/search/author/clusters/A-1456-abcs</t>
   </si>
 </sst>
 </file>
@@ -908,7 +908,7 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1781,7 +1781,7 @@
     </row>
     <row r="29" spans="1:12" ht="120">
       <c r="A29" s="6" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>122</v>
@@ -1790,7 +1790,7 @@
         <v>13</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>0</v>
@@ -1800,7 +1800,7 @@
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
       <c r="J29" s="10" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="K29" s="7" t="s">
         <v>80</v>
@@ -1809,7 +1809,7 @@
     </row>
     <row r="30" spans="1:12" ht="120">
       <c r="A30" s="6" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B30" s="10" t="s">
         <v>123</v>
@@ -1818,7 +1818,7 @@
         <v>13</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>0</v>
@@ -1828,7 +1828,7 @@
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
       <c r="J30" s="10" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="K30" s="7" t="s">
         <v>80</v>
@@ -1837,16 +1837,16 @@
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="6" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>0</v>
@@ -1863,16 +1863,16 @@
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="6" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>0</v>
@@ -1889,10 +1889,10 @@
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="6" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
WAT api scripts automation
</commit_message>
<xml_diff>
--- a/src/test/test-data/WATTestData.xlsx
+++ b/src/test/test-data/WATTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="139">
   <si>
     <t>GET</t>
   </si>
@@ -124,9 +124,6 @@
   </si>
   <si>
     <t>Verify that user is able to search for author cluster using only Last name</t>
-  </si>
-  <si>
-    <t>/recommend/search/author/typeahead/name</t>
   </si>
   <si>
     <t>status=200</t>
@@ -458,6 +455,9 @@
   </si>
   <si>
     <t>/recommend/search/author/clusters/A-1456-abcs</t>
+  </si>
+  <si>
+    <t>/recommend/search/author/typeahead/lastName</t>
   </si>
 </sst>
 </file>
@@ -907,7 +907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
@@ -967,7 +967,7 @@
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" ht="135">
       <c r="A2" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>15</v>
@@ -988,21 +988,21 @@
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
       <c r="J2" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="4" customFormat="1">
       <c r="A3" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>13</v>
@@ -1020,19 +1020,19 @@
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
       <c r="J3" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K3" s="9"/>
       <c r="L3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>13</v>
@@ -1045,21 +1045,21 @@
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="J4" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K4" s="9"/>
       <c r="L4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>16</v>
@@ -1080,16 +1080,16 @@
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K5" s="9"/>
       <c r="L5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>18</v>
@@ -1114,12 +1114,12 @@
       </c>
       <c r="K6" s="16"/>
       <c r="L6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>22</v>
@@ -1135,23 +1135,23 @@
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>25</v>
@@ -1176,12 +1176,12 @@
       </c>
       <c r="K8" s="9"/>
       <c r="L8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>26</v>
@@ -1206,15 +1206,15 @@
       </c>
       <c r="K9" s="9"/>
       <c r="L9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="164.25">
       <c r="A10" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>13</v>
@@ -1232,18 +1232,18 @@
       <c r="H10" s="10"/>
       <c r="I10" s="15"/>
       <c r="J10" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="K10" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="K10" s="12" t="s">
-        <v>97</v>
-      </c>
       <c r="L10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30">
       <c r="A11" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>28</v>
@@ -1267,13 +1267,13 @@
         <v>29</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L11" s="9"/>
     </row>
     <row r="12" spans="1:12" ht="30">
       <c r="A12" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B12" s="20" t="s">
         <v>33</v>
@@ -1289,24 +1289,24 @@
       </c>
       <c r="F12" s="22"/>
       <c r="G12" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H12" s="22"/>
       <c r="I12" s="22"/>
       <c r="J12" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K12" s="18"/>
       <c r="L12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>13</v>
@@ -1319,24 +1319,24 @@
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K13" s="9"/>
       <c r="L13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>13</v>
@@ -1349,24 +1349,24 @@
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
       <c r="J14" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K14" s="9"/>
       <c r="L14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>13</v>
@@ -1379,24 +1379,24 @@
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
       <c r="J15" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K15" s="9"/>
       <c r="L15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="30">
       <c r="A16" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>13</v>
@@ -1409,24 +1409,24 @@
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K16" s="9"/>
       <c r="L16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="30">
       <c r="A17" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>13</v>
@@ -1439,24 +1439,24 @@
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
       <c r="J17" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K17" s="16"/>
       <c r="L17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>13</v>
@@ -1469,7 +1469,7 @@
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
@@ -1478,15 +1478,15 @@
       </c>
       <c r="K18" s="9"/>
       <c r="L18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>13</v>
@@ -1499,7 +1499,7 @@
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
@@ -1508,15 +1508,15 @@
       </c>
       <c r="K19" s="9"/>
       <c r="L19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>13</v>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
@@ -1538,15 +1538,15 @@
       </c>
       <c r="K20" s="9"/>
       <c r="L20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>13</v>
@@ -1559,7 +1559,7 @@
       </c>
       <c r="F21" s="10"/>
       <c r="G21" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
@@ -1568,171 +1568,171 @@
       </c>
       <c r="K21" s="9"/>
       <c r="L21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
       <c r="J22" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K22" s="9"/>
       <c r="L22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
       <c r="J23" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K23" s="9"/>
       <c r="L23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="30">
       <c r="A24" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
       <c r="J24" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K24" s="9"/>
       <c r="L24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="30">
       <c r="A25" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="10"/>
       <c r="J25" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K25" s="9"/>
       <c r="L25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="30">
       <c r="A26" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F26" s="10"/>
       <c r="G26" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
       <c r="J26" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K26" s="9"/>
       <c r="L26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>34</v>
+        <v>138</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>0</v>
@@ -1742,55 +1742,55 @@
       <c r="H27" s="10"/>
       <c r="I27" s="10"/>
       <c r="J27" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K27" s="9"/>
       <c r="L27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="30">
       <c r="A28" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>34</v>
+        <v>138</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F28" s="15"/>
       <c r="G28" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H28" s="15"/>
       <c r="I28" s="15"/>
       <c r="J28" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K28" s="16"/>
       <c r="L28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="120">
       <c r="A29" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>0</v>
@@ -1800,25 +1800,27 @@
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
       <c r="J29" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="L29" s="9"/>
+        <v>79</v>
+      </c>
+      <c r="L29" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="30" spans="1:12" ht="120">
       <c r="A30" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>0</v>
@@ -1828,25 +1830,27 @@
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
       <c r="J30" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="L30" s="9"/>
+        <v>79</v>
+      </c>
+      <c r="L30" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>0</v>
@@ -1859,20 +1863,22 @@
         <v>24</v>
       </c>
       <c r="K31" s="9"/>
-      <c r="L31" s="9"/>
+      <c r="L31" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>0</v>
@@ -1885,20 +1891,22 @@
         <v>24</v>
       </c>
       <c r="K32" s="9"/>
-      <c r="L32" s="9"/>
+      <c r="L32" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>0</v>
@@ -1911,7 +1919,9 @@
         <v>24</v>
       </c>
       <c r="K33" s="9"/>
-      <c r="L33" s="9"/>
+      <c r="L33" t="s">
+        <v>113</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
API new test cases for WAT
</commit_message>
<xml_diff>
--- a/src/test/test-data/WATTestData.xlsx
+++ b/src/test/test-data/WATTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="172">
   <si>
     <t>GET</t>
   </si>
@@ -455,6 +455,108 @@
   </si>
   <si>
     <t>/recommend/search/author/typeahead/lastName</t>
+  </si>
+  <si>
+    <t>/recommend/search/author/24303705</t>
+  </si>
+  <si>
+    <t>Verify that Author metada should not display for invalid Author id</t>
+  </si>
+  <si>
+    <t>/recommend/search/author/a1b345asdjf</t>
+  </si>
+  <si>
+    <t>Verify that  Author metadata should display ORCID for given Author id</t>
+  </si>
+  <si>
+    <t>Verify that  Author metadata should display RID for given Author id</t>
+  </si>
+  <si>
+    <t>/recommend/search/author/80453160</t>
+  </si>
+  <si>
+    <t>Verify that Author metadata should contain following fields, authorId. firstName, lastName, alternativeName, rid, location, primaryAffiliation, department, affiliations, totalTimesCited, hIndex</t>
+  </si>
+  <si>
+    <t>status=400</t>
+  </si>
+  <si>
+    <t>status=200||authorId=24303705||orcid=0000-0002-6423-7213</t>
+  </si>
+  <si>
+    <t>status=200||authorId=80453160||rid=A-9832-2009</t>
+  </si>
+  <si>
+    <t>authorId=80453160||firstName=J M||lastName=TRANQUADA||alternativeName=TRANQUADA, JOHN||orcid=0000-0002-6423-7213||location=UPTON, NY, USA||primaryAffiliation=BROOKHAVEN NATL LAB||department=CONDENSED MATTER PHYS &amp; MAT SCI DEPT||affiliations=BROOKHAVEN NATL LABS||totalTimesCited=9165||hIndex=50</t>
+  </si>
+  <si>
+    <t>WAT-535</t>
+  </si>
+  <si>
+    <t>WAT-426</t>
+  </si>
+  <si>
+    <t>WAT-427</t>
+  </si>
+  <si>
+    <t>WAT-438</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>WAT-429</t>
+  </si>
+  <si>
+    <t>status=200||authorId=80453160||affiliations=BROOKHAVEN NATL LABS</t>
+  </si>
+  <si>
+    <t>WAT-430</t>
+  </si>
+  <si>
+    <t>status=200||authorId=24303705||alternativeName=FABBRI, F.</t>
+  </si>
+  <si>
+    <t>Verify that Author metadata should display metrics info for given Author id i.e. totalTimesCited count and hIndex count</t>
+  </si>
+  <si>
+    <t>WAT-434</t>
+  </si>
+  <si>
+    <t>status=200||authorId=24303705||totalTimesCited=80186||hIndex=91</t>
+  </si>
+  <si>
+    <t>status=200||authorId=24303705</t>
+  </si>
+  <si>
+    <t>Verify that Author metadata  should display organizations for given Author id</t>
+  </si>
+  <si>
+    <t>Verify that Author metadata should display alternative names for given Author id</t>
+  </si>
+  <si>
+    <t>Verify that Author metadata results should display using valid country, affiliation and journal for given Author id</t>
+  </si>
+  <si>
+    <t>?country=USA&amp;affiliation=BROOKHAVEN&amp;journal=physics</t>
+  </si>
+  <si>
+    <t>status=200||location=USA||affiliations=BROOKHAVEN</t>
+  </si>
+  <si>
+    <t>Verify that Author metadata results should display using Invalid country, valid affiliation and valid journal for given Author id</t>
+  </si>
+  <si>
+    <t>?country=INDIA&amp;affiliation=BROOKHAVEN&amp;journal=physics</t>
+  </si>
+  <si>
+    <t>status=200||authorId=80453160</t>
+  </si>
+  <si>
+    <t>WAT-537</t>
+  </si>
+  <si>
+    <t>WAT-538</t>
   </si>
 </sst>
 </file>
@@ -902,10 +1004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -919,8 +1021,8 @@
     <col min="7" max="7" width="42.85546875" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="14" style="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="19.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="59.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="32" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="74.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="36.42578125" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -990,7 +1092,9 @@
       <c r="K2" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="L2"/>
+      <c r="L2" s="9" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="3" spans="1:12" s="4" customFormat="1">
       <c r="A3" s="11" t="s">
@@ -1018,7 +1122,9 @@
         <v>34</v>
       </c>
       <c r="K3" s="9"/>
-      <c r="L3"/>
+      <c r="L3" s="9" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="11" t="s">
@@ -1046,6 +1152,9 @@
         <v>86</v>
       </c>
       <c r="K4" s="9"/>
+      <c r="L4" s="9" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="11" t="s">
@@ -1073,6 +1182,9 @@
         <v>112</v>
       </c>
       <c r="K5" s="9"/>
+      <c r="L5" s="9" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="11" t="s">
@@ -1100,6 +1212,9 @@
         <v>21</v>
       </c>
       <c r="K6" s="16"/>
+      <c r="L6" s="9" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="11" t="s">
@@ -1129,6 +1244,9 @@
       <c r="K7" s="9" t="s">
         <v>90</v>
       </c>
+      <c r="L7" s="9" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="11" t="s">
@@ -1156,6 +1274,9 @@
         <v>24</v>
       </c>
       <c r="K8" s="9"/>
+      <c r="L8" s="9" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="11" t="s">
@@ -1183,6 +1304,9 @@
         <v>24</v>
       </c>
       <c r="K9" s="9"/>
+      <c r="L9" s="9" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="164.25">
       <c r="A10" s="11" t="s">
@@ -1212,6 +1336,9 @@
       <c r="K10" s="12" t="s">
         <v>96</v>
       </c>
+      <c r="L10" s="9" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="11" spans="1:12" ht="30">
       <c r="A11" s="6" t="s">
@@ -1243,7 +1370,7 @@
       </c>
       <c r="L11" s="9"/>
     </row>
-    <row r="12" spans="1:12" ht="30">
+    <row r="12" spans="1:12">
       <c r="A12" s="6" t="s">
         <v>100</v>
       </c>
@@ -1269,6 +1396,9 @@
         <v>56</v>
       </c>
       <c r="K12" s="18"/>
+      <c r="L12" s="9" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="6" t="s">
@@ -1296,6 +1426,9 @@
         <v>59</v>
       </c>
       <c r="K13" s="9"/>
+      <c r="L13" s="9" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" s="6" t="s">
@@ -1323,6 +1456,9 @@
         <v>104</v>
       </c>
       <c r="K14" s="9"/>
+      <c r="L14" s="9" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="6" t="s">
@@ -1350,8 +1486,11 @@
         <v>63</v>
       </c>
       <c r="K15" s="9"/>
-    </row>
-    <row r="16" spans="1:12" ht="30">
+      <c r="L15" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="6" t="s">
         <v>106</v>
       </c>
@@ -1377,8 +1516,11 @@
         <v>65</v>
       </c>
       <c r="K16" s="9"/>
-    </row>
-    <row r="17" spans="1:11" ht="30">
+      <c r="L16" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="6" t="s">
         <v>107</v>
       </c>
@@ -1404,8 +1546,11 @@
         <v>69</v>
       </c>
       <c r="K17" s="16"/>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="L17" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="6" t="s">
         <v>108</v>
       </c>
@@ -1431,8 +1576,11 @@
         <v>24</v>
       </c>
       <c r="K18" s="9"/>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="L18" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="6" t="s">
         <v>109</v>
       </c>
@@ -1458,8 +1606,11 @@
         <v>24</v>
       </c>
       <c r="K19" s="9"/>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="L19" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="6" t="s">
         <v>110</v>
       </c>
@@ -1485,8 +1636,11 @@
         <v>24</v>
       </c>
       <c r="K20" s="9"/>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="L20" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="6" t="s">
         <v>111</v>
       </c>
@@ -1512,8 +1666,11 @@
         <v>24</v>
       </c>
       <c r="K21" s="9"/>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="L21" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="6" t="s">
         <v>113</v>
       </c>
@@ -1539,8 +1696,11 @@
         <v>34</v>
       </c>
       <c r="K22" s="9"/>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="L22" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="6" t="s">
         <v>114</v>
       </c>
@@ -1566,8 +1726,11 @@
         <v>49</v>
       </c>
       <c r="K23" s="9"/>
-    </row>
-    <row r="24" spans="1:11" ht="30">
+      <c r="L23" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="30">
       <c r="A24" s="6" t="s">
         <v>115</v>
       </c>
@@ -1593,8 +1756,11 @@
         <v>50</v>
       </c>
       <c r="K24" s="9"/>
-    </row>
-    <row r="25" spans="1:11" ht="30">
+      <c r="L24" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="30">
       <c r="A25" s="6" t="s">
         <v>116</v>
       </c>
@@ -1620,8 +1786,11 @@
         <v>51</v>
       </c>
       <c r="K25" s="9"/>
-    </row>
-    <row r="26" spans="1:11" ht="30">
+      <c r="L25" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="30">
       <c r="A26" s="6" t="s">
         <v>117</v>
       </c>
@@ -1647,8 +1816,11 @@
         <v>53</v>
       </c>
       <c r="K26" s="9"/>
-    </row>
-    <row r="27" spans="1:11">
+      <c r="L26" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" s="6" t="s">
         <v>118</v>
       </c>
@@ -1672,8 +1844,11 @@
         <v>34</v>
       </c>
       <c r="K27" s="9"/>
-    </row>
-    <row r="28" spans="1:11" ht="30">
+      <c r="L27" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="30">
       <c r="A28" s="6" t="s">
         <v>119</v>
       </c>
@@ -1699,8 +1874,11 @@
         <v>34</v>
       </c>
       <c r="K28" s="16"/>
-    </row>
-    <row r="29" spans="1:11" ht="120">
+      <c r="L28" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="105">
       <c r="A29" s="6" t="s">
         <v>127</v>
       </c>
@@ -1726,8 +1904,11 @@
       <c r="K29" s="7" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" ht="120">
+      <c r="L29" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="105">
       <c r="A30" s="6" t="s">
         <v>129</v>
       </c>
@@ -1753,8 +1934,11 @@
       <c r="K30" s="7" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="31" spans="1:11">
+      <c r="L30" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" s="6" t="s">
         <v>128</v>
       </c>
@@ -1778,8 +1962,11 @@
         <v>24</v>
       </c>
       <c r="K31" s="9"/>
-    </row>
-    <row r="32" spans="1:11">
+      <c r="L31" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32" s="6" t="s">
         <v>130</v>
       </c>
@@ -1803,8 +1990,11 @@
         <v>24</v>
       </c>
       <c r="K32" s="9"/>
-    </row>
-    <row r="33" spans="1:11">
+      <c r="L32" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" s="6" t="s">
         <v>131</v>
       </c>
@@ -1828,9 +2018,269 @@
         <v>24</v>
       </c>
       <c r="K33" s="9"/>
+      <c r="L33" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F34" s="10"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F35" s="10"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="K35" s="9"/>
+      <c r="L35" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F36" s="15"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="K36" s="16"/>
+      <c r="L36" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="180">
+      <c r="A37" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F37" s="10"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="K37" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="L37" s="9"/>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F38" s="10"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F39" s="10"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="30">
+      <c r="A40" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F40" s="10"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="30">
+      <c r="A41" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="K41" s="16"/>
+      <c r="L41" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="30">
+      <c r="A42" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="K42" s="9"/>
+      <c r="L42" s="9"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A36" r:id="rId1" display="http://ent.jira.int.thomsonreuters.com/browse/WAT-535"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
WAT API automation test scripts
</commit_message>
<xml_diff>
--- a/src/test/test-data/WATTestData.xlsx
+++ b/src/test/test-data/WATTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="177">
   <si>
     <t>GET</t>
   </si>
@@ -557,6 +557,21 @@
   </si>
   <si>
     <t>WAT-538</t>
+  </si>
+  <si>
+    <t>lastName||firstName</t>
+  </si>
+  <si>
+    <t>status=200||hits[0].primaryName=(WAT-430_lastName)||hits[0].primaryName=(WAT-430_firstName)</t>
+  </si>
+  <si>
+    <t>orcid</t>
+  </si>
+  <si>
+    <t>Verify that author cluster details primary name should match with author metadata last name and first name</t>
+  </si>
+  <si>
+    <t>WAT-541</t>
   </si>
 </sst>
 </file>
@@ -1004,10 +1019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2045,7 +2060,9 @@
       <c r="J34" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="K34" s="9"/>
+      <c r="K34" s="9" t="s">
+        <v>174</v>
+      </c>
       <c r="L34" s="9" t="s">
         <v>153</v>
       </c>
@@ -2185,7 +2202,9 @@
       <c r="J39" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="K39" s="9"/>
+      <c r="K39" s="9" t="s">
+        <v>172</v>
+      </c>
       <c r="L39" s="9" t="s">
         <v>153</v>
       </c>
@@ -2274,7 +2293,39 @@
         <v>169</v>
       </c>
       <c r="K42" s="9"/>
-      <c r="L42" s="9"/>
+      <c r="L42" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="30">
+      <c r="A43" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F43" s="10"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="J43" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="K43" s="9"/>
+      <c r="L43" t="s">
+        <v>153</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
WAT service changed from 1PRecommend to WOSAUTHORRECOMMEND
</commit_message>
<xml_diff>
--- a/src/test/test-data/WATTestData.xlsx
+++ b/src/test/test-data/WATTestData.xlsx
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>DEPENDENCYTESTS</t>
-  </si>
-  <si>
-    <t>1PRECOMMEND</t>
   </si>
   <si>
     <t>/recommend/search/author/clusters</t>
@@ -596,6 +593,9 @@
   </si>
   <si>
     <t>WAT-572</t>
+  </si>
+  <si>
+    <t>WOSAUTHORRECOMMEND</t>
   </si>
 </sst>
 </file>
@@ -1045,15 +1045,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:A45"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="90.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="80.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1105,772 +1105,772 @@
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" ht="135">
       <c r="A2" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>13</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>14</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
       <c r="J2" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="4" customFormat="1">
       <c r="A3" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="10"/>
       <c r="G3" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
       <c r="J3" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K3" s="9"/>
       <c r="L3" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="J4" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K4" s="9"/>
       <c r="L4" s="9" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="30">
       <c r="A5" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="9" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="30">
       <c r="A6" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>13</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>14</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F6" s="15"/>
       <c r="G6" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
       <c r="J6" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K6" s="16"/>
       <c r="L6" s="9" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="30">
       <c r="A7" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K8" s="9"/>
       <c r="L8" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K9" s="9"/>
       <c r="L9" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="164.25">
       <c r="A10" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="15"/>
       <c r="J10" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="K10" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="K10" s="12" t="s">
-        <v>96</v>
-      </c>
       <c r="L10" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30">
       <c r="A11" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L11" s="9"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="D12" s="20" t="s">
         <v>13</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>14</v>
       </c>
       <c r="E12" s="21" t="s">
         <v>0</v>
       </c>
       <c r="F12" s="22"/>
       <c r="G12" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H12" s="22"/>
       <c r="I12" s="22"/>
       <c r="J12" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K12" s="18"/>
       <c r="L12" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C13" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K13" s="9"/>
       <c r="L13" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
       <c r="J14" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K14" s="9"/>
       <c r="L14" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
       <c r="J15" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K15" s="9"/>
       <c r="L15" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K16" s="9"/>
       <c r="L16" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C17" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="D17" s="13" t="s">
         <v>13</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>14</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
       <c r="J17" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K17" s="16"/>
       <c r="L17" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
       <c r="J18" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K18" s="9"/>
       <c r="L18" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C19" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
       <c r="J19" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K19" s="9"/>
       <c r="L19" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C20" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
       <c r="J20" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K20" s="9"/>
       <c r="L20" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C21" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F21" s="10"/>
       <c r="G21" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
       <c r="J21" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K21" s="9"/>
       <c r="L21" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
       <c r="J22" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K22" s="9"/>
       <c r="L22" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
       <c r="J23" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K23" s="9"/>
       <c r="L23" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="30">
       <c r="A24" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
       <c r="J24" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K24" s="9"/>
       <c r="L24" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="30">
       <c r="A25" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="10"/>
       <c r="J25" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K25" s="9"/>
       <c r="L25" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="30">
       <c r="A26" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F26" s="10"/>
       <c r="G26" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
       <c r="J26" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K26" s="9"/>
       <c r="L26" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>0</v>
@@ -1880,55 +1880,55 @@
       <c r="H27" s="10"/>
       <c r="I27" s="10"/>
       <c r="J27" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K27" s="9"/>
       <c r="L27" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="30">
       <c r="A28" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F28" s="15"/>
       <c r="G28" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H28" s="15"/>
       <c r="I28" s="15"/>
       <c r="J28" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K28" s="16"/>
       <c r="L28" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="105">
       <c r="A29" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>0</v>
@@ -1938,27 +1938,27 @@
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
       <c r="J29" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L29" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="105">
       <c r="A30" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>0</v>
@@ -1968,27 +1968,27 @@
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
       <c r="J30" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L30" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>0</v>
@@ -1998,25 +1998,25 @@
       <c r="H31" s="10"/>
       <c r="I31" s="10"/>
       <c r="J31" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K31" s="9"/>
       <c r="L31" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>0</v>
@@ -2026,25 +2026,25 @@
       <c r="H32" s="10"/>
       <c r="I32" s="10"/>
       <c r="J32" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K32" s="9"/>
       <c r="L32" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>0</v>
@@ -2054,25 +2054,25 @@
       <c r="H33" s="10"/>
       <c r="I33" s="10"/>
       <c r="J33" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K33" s="9"/>
       <c r="L33" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>0</v>
@@ -2082,27 +2082,27 @@
       <c r="H34" s="10"/>
       <c r="I34" s="10"/>
       <c r="J34" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K34" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L34" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B35" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D35" s="8" t="s">
         <v>139</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>140</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>0</v>
@@ -2112,25 +2112,25 @@
       <c r="H35" s="10"/>
       <c r="I35" s="10"/>
       <c r="J35" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K35" s="9"/>
       <c r="L35" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B36" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="D36" s="13" t="s">
         <v>142</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>143</v>
       </c>
       <c r="E36" s="11" t="s">
         <v>0</v>
@@ -2140,25 +2140,25 @@
       <c r="H36" s="15"/>
       <c r="I36" s="15"/>
       <c r="J36" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K36" s="16"/>
       <c r="L36" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="180">
       <c r="A37" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>0</v>
@@ -2168,25 +2168,25 @@
       <c r="H37" s="10"/>
       <c r="I37" s="10"/>
       <c r="J37" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K37" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L37" s="9"/>
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>0</v>
@@ -2196,25 +2196,25 @@
       <c r="H38" s="10"/>
       <c r="I38" s="10"/>
       <c r="J38" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K38" s="9"/>
       <c r="L38" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>0</v>
@@ -2224,27 +2224,27 @@
       <c r="H39" s="10"/>
       <c r="I39" s="10"/>
       <c r="J39" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K39" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L39" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="30">
       <c r="A40" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>0</v>
@@ -2254,85 +2254,85 @@
       <c r="H40" s="10"/>
       <c r="I40" s="10"/>
       <c r="J40" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K40" s="9"/>
       <c r="L40" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="30">
       <c r="A41" s="16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E41" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F41" s="15"/>
       <c r="G41" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H41" s="15"/>
       <c r="I41" s="15"/>
       <c r="J41" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K41" s="16"/>
       <c r="L41" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="30">
       <c r="A42" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F42" s="10"/>
       <c r="G42" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H42" s="10"/>
       <c r="I42" s="10"/>
       <c r="J42" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K42" s="9"/>
       <c r="L42" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="30">
       <c r="A43" s="16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>13</v>
+        <v>184</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E43" s="16" t="s">
         <v>0</v>
@@ -2341,68 +2341,68 @@
       <c r="G43" s="16"/>
       <c r="H43" s="15"/>
       <c r="I43" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J43" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K43" s="16"/>
       <c r="L43" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="44" spans="1:12">
       <c r="A44" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C44" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D44" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F44" s="10"/>
       <c r="G44" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H44" s="10"/>
       <c r="I44" s="10"/>
       <c r="J44" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K44" s="10"/>
       <c r="L44" s="9"/>
     </row>
     <row r="45" spans="1:12" ht="30">
       <c r="A45" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C45" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D45" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F45" s="10"/>
       <c r="G45" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H45" s="10"/>
       <c r="I45" s="10"/>
       <c r="J45" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K45" s="9"/>
       <c r="L45" s="9"/>

</xml_diff>

<commit_message>
WAT API testcases for NEON-1187
</commit_message>
<xml_diff>
--- a/src/test/test-data/WATTestData.xlsx
+++ b/src/test/test-data/WATTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="202">
   <si>
     <t>GET</t>
   </si>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>?authorId=80451360&amp;authorId=80453185</t>
-  </si>
-  <si>
-    <t>?name=Smith,J,G&amp;country=USA&amp;affiliation=UNIV COLORADO&amp;journal=physics&amp;offset=0&amp;limit=10</t>
   </si>
   <si>
     <t>Verify that user is able to search for author cluster using only Last name</t>
@@ -596,6 +593,60 @@
   </si>
   <si>
     <t>status=200||authorId=0</t>
+  </si>
+  <si>
+    <t>?name=Smith&amp;country=USA&amp;affiliation=UNIV COLORADO&amp;journal=physics&amp;offset=0&amp;limit=10</t>
+  </si>
+  <si>
+    <t>status=200||hits.primaryName=Smith||hits.location=USA||hits.affiliation=UNIV COLORADO</t>
+  </si>
+  <si>
+    <t>WAT-410</t>
+  </si>
+  <si>
+    <t>Verify that user should be able to filter values for an author using provided filter name,affiliation,category</t>
+  </si>
+  <si>
+    <t>?name=manalang&amp;country=USA&amp;affiliation=UNIV MISSOURI&amp;filter=name&amp;filter=affiliation&amp;filter=category</t>
+  </si>
+  <si>
+    <t>status=200||filters.primaryName=manalang||filters.category=PEDIATRICSHEMATOLOGY|||filters.affiliation=UNIV MISSOURI</t>
+  </si>
+  <si>
+    <t>WAT-411</t>
+  </si>
+  <si>
+    <t>?name=manalang&amp;filter=name</t>
+  </si>
+  <si>
+    <t>status=200||hits.primaryName=manalang||filters.primaryName=manalang</t>
+  </si>
+  <si>
+    <t>?name=bhavya&amp;affiliation=indian&amp;filter=affiliation</t>
+  </si>
+  <si>
+    <t>status=200||hits.primaryName=bhavya||filters.affiliation=indian</t>
+  </si>
+  <si>
+    <t>?name=bhavya&amp;category=AGRICULTURE&amp;filter=category</t>
+  </si>
+  <si>
+    <t>status=200||hits.primaryName=bhavya||filters.category=AGRICULTURE</t>
+  </si>
+  <si>
+    <t>WAT-412</t>
+  </si>
+  <si>
+    <t>Verify that user should be able to filter values for an author using 'category' filter</t>
+  </si>
+  <si>
+    <t>WAT-414</t>
+  </si>
+  <si>
+    <t>Verify that user should be able to filter values for an author using 'name' filter</t>
+  </si>
+  <si>
+    <t>Verify that user should be able to filter values for an author using 'affiliation' filter</t>
   </si>
 </sst>
 </file>
@@ -1043,10 +1094,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L45"/>
+  <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E30" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1105,48 +1156,48 @@
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" ht="135">
       <c r="A2" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="7" t="s">
-        <v>29</v>
+        <v>184</v>
       </c>
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
       <c r="J2" s="14" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="4" customFormat="1">
       <c r="A3" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>0</v>
@@ -1158,55 +1209,55 @@
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
       <c r="J3" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K3" s="9"/>
       <c r="L3" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="J4" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K4" s="9"/>
       <c r="L4" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>0</v>
@@ -1218,25 +1269,25 @@
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>0</v>
@@ -1252,53 +1303,53 @@
       </c>
       <c r="K6" s="16"/>
       <c r="L6" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>0</v>
@@ -1314,21 +1365,21 @@
       </c>
       <c r="K8" s="9"/>
       <c r="L8" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>0</v>
@@ -1344,21 +1395,21 @@
       </c>
       <c r="K9" s="9"/>
       <c r="L9" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="164.25">
       <c r="A10" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>0</v>
@@ -1370,27 +1421,27 @@
       <c r="H10" s="10"/>
       <c r="I10" s="15"/>
       <c r="J10" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="K10" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="K10" s="12" t="s">
-        <v>90</v>
-      </c>
       <c r="L10" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30">
       <c r="A11" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>0</v>
@@ -1405,209 +1456,209 @@
         <v>26</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L11" s="9"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E12" s="21" t="s">
         <v>0</v>
       </c>
       <c r="F12" s="22"/>
       <c r="G12" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H12" s="22"/>
       <c r="I12" s="22"/>
       <c r="J12" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K12" s="18"/>
       <c r="L12" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K13" s="9"/>
       <c r="L13" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
       <c r="J14" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K14" s="9"/>
       <c r="L14" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
       <c r="J15" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K15" s="9"/>
       <c r="L15" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K16" s="9"/>
       <c r="L16" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
       <c r="J17" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K17" s="16"/>
       <c r="L17" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
@@ -1616,28 +1667,28 @@
       </c>
       <c r="K18" s="9"/>
       <c r="L18" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
@@ -1646,28 +1697,28 @@
       </c>
       <c r="K19" s="9"/>
       <c r="L19" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
@@ -1676,28 +1727,28 @@
       </c>
       <c r="K20" s="9"/>
       <c r="L20" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F21" s="10"/>
       <c r="G21" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
@@ -1706,171 +1757,171 @@
       </c>
       <c r="K21" s="9"/>
       <c r="L21" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>169</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>170</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
       <c r="J22" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K22" s="9"/>
       <c r="L22" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
       <c r="J23" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K23" s="9"/>
       <c r="L23" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="30">
       <c r="A24" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
       <c r="J24" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K24" s="9"/>
       <c r="L24" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="30">
       <c r="A25" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="10"/>
       <c r="J25" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K25" s="9"/>
       <c r="L25" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="30">
       <c r="A26" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F26" s="10"/>
       <c r="G26" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
       <c r="J26" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K26" s="9"/>
       <c r="L26" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>0</v>
@@ -1880,55 +1931,55 @@
       <c r="H27" s="10"/>
       <c r="I27" s="10"/>
       <c r="J27" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K27" s="9"/>
       <c r="L27" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="30">
       <c r="A28" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F28" s="15"/>
       <c r="G28" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H28" s="15"/>
       <c r="I28" s="15"/>
       <c r="J28" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K28" s="16"/>
       <c r="L28" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="105">
       <c r="A29" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>0</v>
@@ -1938,27 +1989,27 @@
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
       <c r="J29" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L29" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="105">
       <c r="A30" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>0</v>
@@ -1968,27 +2019,27 @@
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
       <c r="J30" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L30" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>0</v>
@@ -2002,21 +2053,21 @@
       </c>
       <c r="K31" s="9"/>
       <c r="L31" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>0</v>
@@ -2030,21 +2081,21 @@
       </c>
       <c r="K32" s="9"/>
       <c r="L32" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>0</v>
@@ -2058,21 +2109,21 @@
       </c>
       <c r="K33" s="9"/>
       <c r="L33" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>0</v>
@@ -2082,27 +2133,27 @@
       <c r="H34" s="10"/>
       <c r="I34" s="10"/>
       <c r="J34" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K34" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L34" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>0</v>
@@ -2112,25 +2163,25 @@
       <c r="H35" s="10"/>
       <c r="I35" s="10"/>
       <c r="J35" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K35" s="9"/>
       <c r="L35" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E36" s="11" t="s">
         <v>0</v>
@@ -2140,25 +2191,25 @@
       <c r="H36" s="15"/>
       <c r="I36" s="15"/>
       <c r="J36" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K36" s="16"/>
       <c r="L36" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="180">
       <c r="A37" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>0</v>
@@ -2168,25 +2219,25 @@
       <c r="H37" s="10"/>
       <c r="I37" s="10"/>
       <c r="J37" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K37" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L37" s="9"/>
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>0</v>
@@ -2196,25 +2247,25 @@
       <c r="H38" s="10"/>
       <c r="I38" s="10"/>
       <c r="J38" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K38" s="9"/>
       <c r="L38" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>0</v>
@@ -2224,27 +2275,27 @@
       <c r="H39" s="10"/>
       <c r="I39" s="10"/>
       <c r="J39" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K39" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L39" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="30">
       <c r="A40" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>0</v>
@@ -2254,85 +2305,85 @@
       <c r="H40" s="10"/>
       <c r="I40" s="10"/>
       <c r="J40" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K40" s="9"/>
       <c r="L40" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="30">
       <c r="A41" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E41" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F41" s="15"/>
       <c r="G41" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H41" s="15"/>
       <c r="I41" s="15"/>
       <c r="J41" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K41" s="16"/>
       <c r="L41" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="30">
       <c r="A42" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F42" s="10"/>
       <c r="G42" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H42" s="10"/>
       <c r="I42" s="10"/>
       <c r="J42" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K42" s="9"/>
       <c r="L42" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="30">
       <c r="A43" s="16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E43" s="16" t="s">
         <v>0</v>
@@ -2341,73 +2392,185 @@
       <c r="G43" s="16"/>
       <c r="H43" s="15"/>
       <c r="I43" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J43" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K43" s="16"/>
       <c r="L43" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:12">
       <c r="A44" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F44" s="10"/>
       <c r="G44" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H44" s="10"/>
       <c r="I44" s="10"/>
       <c r="J44" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K44" s="10"/>
       <c r="L44" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="30">
       <c r="A45" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F45" s="10"/>
       <c r="G45" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H45" s="10"/>
       <c r="I45" s="10"/>
       <c r="J45" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K45" s="9"/>
       <c r="L45" s="9"/>
+    </row>
+    <row r="46" spans="1:12" ht="45">
+      <c r="A46" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="K46" s="9"/>
+      <c r="L46" s="9"/>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
+      <c r="J47" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="K47" s="9"/>
+      <c r="L47" s="9"/>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="K48" s="9"/>
+      <c r="L48" s="9"/>
+    </row>
+    <row r="49" spans="1:12" ht="30">
+      <c r="A49" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="K49" s="9"/>
+      <c r="L49" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
WAT new script implementation
</commit_message>
<xml_diff>
--- a/src/test/test-data/WATTestData.xlsx
+++ b/src/test/test-data/WATTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="207">
   <si>
     <t>GET</t>
   </si>
@@ -647,6 +647,21 @@
   </si>
   <si>
     <t>Verify that user should be able to filter values for an author using 'affiliation' filter</t>
+  </si>
+  <si>
+    <t>?name=wang&amp;affiliation=china&amp;filter=name&amp;category=physics&amp;filter=affiliation&amp;filter=catagory&amp;sort=year&amp;order=asc&amp;limit=10</t>
+  </si>
+  <si>
+    <t>status=200||hits.primaryName=wang||filters.category=physics||hits.affiliation=china</t>
+  </si>
+  <si>
+    <t>hits[0].publicationYearRangeMin||hits.publicationYearRangeMax</t>
+  </si>
+  <si>
+    <t>Verify that user should be able to filter values for a set of authors  provided with all the mandatory inputs along with sorting given an order</t>
+  </si>
+  <si>
+    <t>WAT-413</t>
   </si>
 </sst>
 </file>
@@ -1094,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2572,6 +2587,36 @@
       <c r="K49" s="9"/>
       <c r="L49" s="9"/>
     </row>
+    <row r="50" spans="1:12" ht="45">
+      <c r="A50" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
+      <c r="J50" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="K50" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="L50" s="9"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A36" r:id="rId1" display="http://ent.jira.int.thomsonreuters.com/browse/WAT-535"/>

</xml_diff>

<commit_message>
WAT API new script implementation
</commit_message>
<xml_diff>
--- a/src/test/test-data/WATTestData.xlsx
+++ b/src/test/test-data/WATTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="211">
   <si>
     <t>GET</t>
   </si>
@@ -658,10 +658,22 @@
     <t>hits[0].publicationYearRangeMin||hits.publicationYearRangeMax</t>
   </si>
   <si>
-    <t>Verify that user should be able to filter values for a set of authors  provided with all the mandatory inputs along with sorting given an order</t>
-  </si>
-  <si>
     <t>WAT-413</t>
+  </si>
+  <si>
+    <t>WAT-415</t>
+  </si>
+  <si>
+    <t>Verify that user should be able to filter values for a set of authors  provided with all the mandatory inputs along with sorting using years given an order</t>
+  </si>
+  <si>
+    <t>Verify that user should be able to filter values for a set of authors provided with all the mandatory inputs along with sorting using totalNumberOfPublications given an order</t>
+  </si>
+  <si>
+    <t>?name=wang&amp;affiliation=china&amp;filter=name&amp;category=physics&amp;filter=affiliation&amp;filter=catagory&amp;sort=totalNumberOfPublications&amp;order=asc&amp;limit=10</t>
+  </si>
+  <si>
+    <t>hits[0].totalNumberOfPublications</t>
   </si>
 </sst>
 </file>
@@ -1109,10 +1121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L50"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" topLeftCell="E38" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K51" sqref="K51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2589,10 +2601,10 @@
     </row>
     <row r="50" spans="1:12" ht="45">
       <c r="A50" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C50" s="8" t="s">
         <v>168</v>
@@ -2616,6 +2628,36 @@
         <v>204</v>
       </c>
       <c r="L50" s="9"/>
+    </row>
+    <row r="51" spans="1:12" ht="45">
+      <c r="A51" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="H51" s="10"/>
+      <c r="I51" s="10"/>
+      <c r="J51" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="K51" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="L51" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
API tests code changes
</commit_message>
<xml_diff>
--- a/src/test/test-data/WATTestData.xlsx
+++ b/src/test/test-data/WATTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="211">
   <si>
     <t>GET</t>
   </si>
@@ -472,9 +472,6 @@
     <t>WAT-434</t>
   </si>
   <si>
-    <t>status=200||authorId=24303705||totalTimesCited=80186||hIndex=91</t>
-  </si>
-  <si>
     <t>status=200||authorId=24303705</t>
   </si>
   <si>
@@ -649,9 +646,6 @@
     <t>Verify that user should be able to filter values for an author using 'affiliation' filter</t>
   </si>
   <si>
-    <t>?name=wang&amp;affiliation=china&amp;filter=name&amp;category=physics&amp;filter=affiliation&amp;filter=catagory&amp;sort=year&amp;order=asc&amp;limit=10</t>
-  </si>
-  <si>
     <t>status=200||hits.primaryName=wang||filters.category=physics||hits.affiliation=china</t>
   </si>
   <si>
@@ -670,10 +664,16 @@
     <t>Verify that user should be able to filter values for a set of authors provided with all the mandatory inputs along with sorting using totalNumberOfPublications given an order</t>
   </si>
   <si>
-    <t>?name=wang&amp;affiliation=china&amp;filter=name&amp;category=physics&amp;filter=affiliation&amp;filter=catagory&amp;sort=totalNumberOfPublications&amp;order=asc&amp;limit=10</t>
-  </si>
-  <si>
     <t>hits[0].totalNumberOfPublications</t>
+  </si>
+  <si>
+    <t>?name=wang&amp;affiliation=china&amp;filter=name&amp;category=physics&amp;filter=affiliation&amp;filter=category&amp;filters.category&amp;sort=year&amp;order=asc&amp;limit=10</t>
+  </si>
+  <si>
+    <t>?name=wang&amp;affiliation=china&amp;filter=name&amp;category=physics&amp;filter=affiliation&amp;filter=category&amp;filters.category&amp;sort=totalNumberOfPublications&amp;order=asc&amp;limit=10</t>
+  </si>
+  <si>
+    <t>hits[0].totalTimesCited||hits[0].hIndex</t>
   </si>
 </sst>
 </file>
@@ -1123,8 +1123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E38" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K51" sqref="K51"/>
+    <sheetView tabSelected="1" topLeftCell="E30" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1189,22 +1189,22 @@
         <v>13</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
       <c r="J2" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K2" s="12" t="s">
         <v>72</v>
@@ -1221,10 +1221,10 @@
         <v>76</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>0</v>
@@ -1251,10 +1251,10 @@
         <v>77</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>0</v>
@@ -1281,10 +1281,10 @@
         <v>14</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>0</v>
@@ -1311,10 +1311,10 @@
         <v>16</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>0</v>
@@ -1341,10 +1341,10 @@
         <v>19</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>0</v>
@@ -1373,10 +1373,10 @@
         <v>22</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>0</v>
@@ -1403,10 +1403,10 @@
         <v>23</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>0</v>
@@ -1433,10 +1433,10 @@
         <v>71</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>0</v>
@@ -1465,10 +1465,10 @@
         <v>25</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>0</v>
@@ -1495,10 +1495,10 @@
         <v>29</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E12" s="21" t="s">
         <v>0</v>
@@ -1525,10 +1525,10 @@
         <v>50</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>0</v>
@@ -1555,10 +1555,10 @@
         <v>53</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>0</v>
@@ -1585,10 +1585,10 @@
         <v>54</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>0</v>
@@ -1615,10 +1615,10 @@
         <v>59</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>0</v>
@@ -1645,10 +1645,10 @@
         <v>61</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>0</v>
@@ -1675,10 +1675,10 @@
         <v>66</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>0</v>
@@ -1705,10 +1705,10 @@
         <v>63</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>0</v>
@@ -1735,10 +1735,10 @@
         <v>64</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>0</v>
@@ -1765,10 +1765,10 @@
         <v>65</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>0</v>
@@ -1795,10 +1795,10 @@
         <v>35</v>
       </c>
       <c r="C22" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>168</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>169</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>0</v>
@@ -1825,10 +1825,10 @@
         <v>36</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>0</v>
@@ -1855,10 +1855,10 @@
         <v>37</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>0</v>
@@ -1885,10 +1885,10 @@
         <v>38</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>0</v>
@@ -1915,10 +1915,10 @@
         <v>39</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>0</v>
@@ -1945,10 +1945,10 @@
         <v>40</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>0</v>
@@ -1973,10 +1973,10 @@
         <v>34</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>0</v>
@@ -2003,10 +2003,10 @@
         <v>113</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>0</v>
@@ -2033,10 +2033,10 @@
         <v>114</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>0</v>
@@ -2063,10 +2063,10 @@
         <v>115</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>0</v>
@@ -2091,10 +2091,10 @@
         <v>118</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>0</v>
@@ -2119,10 +2119,10 @@
         <v>119</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>0</v>
@@ -2147,10 +2147,10 @@
         <v>126</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>0</v>
@@ -2163,7 +2163,7 @@
         <v>129</v>
       </c>
       <c r="K34" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L34" s="9" t="s">
         <v>136</v>
@@ -2177,10 +2177,10 @@
         <v>125</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>0</v>
@@ -2190,7 +2190,7 @@
       <c r="H35" s="10"/>
       <c r="I35" s="10"/>
       <c r="J35" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K35" s="9"/>
       <c r="L35" s="9" t="s">
@@ -2205,10 +2205,10 @@
         <v>127</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E36" s="11" t="s">
         <v>0</v>
@@ -2233,10 +2233,10 @@
         <v>128</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>0</v>
@@ -2246,7 +2246,7 @@
       <c r="H37" s="10"/>
       <c r="I37" s="10"/>
       <c r="J37" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K37" s="10" t="s">
         <v>131</v>
@@ -2258,13 +2258,13 @@
         <v>137</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>0</v>
@@ -2286,13 +2286,13 @@
         <v>139</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>0</v>
@@ -2305,7 +2305,7 @@
         <v>140</v>
       </c>
       <c r="K39" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L39" s="9" t="s">
         <v>136</v>
@@ -2319,10 +2319,10 @@
         <v>141</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>0</v>
@@ -2334,35 +2334,37 @@
       <c r="J40" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="K40" s="9"/>
+      <c r="K40" s="9" t="s">
+        <v>210</v>
+      </c>
       <c r="L40" s="9" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="30">
       <c r="A41" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E41" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F41" s="15"/>
       <c r="G41" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H41" s="15"/>
       <c r="I41" s="15"/>
       <c r="J41" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K41" s="16"/>
       <c r="L41" s="9" t="s">
@@ -2371,28 +2373,28 @@
     </row>
     <row r="42" spans="1:12" ht="30">
       <c r="A42" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F42" s="10"/>
       <c r="G42" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H42" s="10"/>
       <c r="I42" s="10"/>
       <c r="J42" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K42" s="9"/>
       <c r="L42" s="9" t="s">
@@ -2401,16 +2403,16 @@
     </row>
     <row r="43" spans="1:12" ht="30">
       <c r="A43" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E43" s="16" t="s">
         <v>0</v>
@@ -2422,7 +2424,7 @@
         <v>139</v>
       </c>
       <c r="J43" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K43" s="16"/>
       <c r="L43" s="16" t="s">
@@ -2431,28 +2433,28 @@
     </row>
     <row r="44" spans="1:12">
       <c r="A44" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F44" s="10"/>
       <c r="G44" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H44" s="10"/>
       <c r="I44" s="10"/>
       <c r="J44" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K44" s="10"/>
       <c r="L44" t="s">
@@ -2461,186 +2463,186 @@
     </row>
     <row r="45" spans="1:12" ht="30">
       <c r="A45" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F45" s="10"/>
       <c r="G45" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H45" s="10"/>
       <c r="I45" s="10"/>
       <c r="J45" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K45" s="9"/>
       <c r="L45" s="9"/>
     </row>
     <row r="46" spans="1:12" ht="45">
       <c r="A46" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="B46" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="B46" s="10" t="s">
-        <v>187</v>
-      </c>
       <c r="C46" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F46" s="10"/>
       <c r="G46" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H46" s="10"/>
       <c r="I46" s="10"/>
       <c r="J46" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K46" s="9"/>
       <c r="L46" s="9"/>
     </row>
     <row r="47" spans="1:12">
       <c r="A47" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F47" s="10"/>
       <c r="G47" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H47" s="10"/>
       <c r="I47" s="10"/>
       <c r="J47" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K47" s="9"/>
       <c r="L47" s="9"/>
     </row>
     <row r="48" spans="1:12">
       <c r="A48" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F48" s="10"/>
       <c r="G48" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H48" s="10"/>
       <c r="I48" s="10"/>
       <c r="J48" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K48" s="9"/>
       <c r="L48" s="9"/>
     </row>
     <row r="49" spans="1:12" ht="30">
       <c r="A49" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F49" s="10"/>
       <c r="G49" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H49" s="10"/>
       <c r="I49" s="10"/>
       <c r="J49" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K49" s="9"/>
       <c r="L49" s="9"/>
     </row>
     <row r="50" spans="1:12" ht="45">
       <c r="A50" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="B50" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="B50" s="10" t="s">
-        <v>207</v>
-      </c>
       <c r="C50" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F50" s="10"/>
       <c r="G50" s="10" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="H50" s="10"/>
       <c r="I50" s="10"/>
       <c r="J50" s="10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="K50" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="L50" s="9"/>
+    </row>
+    <row r="51" spans="1:12" ht="60">
+      <c r="A51" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="L50" s="9"/>
-    </row>
-    <row r="51" spans="1:12" ht="45">
-      <c r="A51" s="9" t="s">
+      <c r="B51" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="B51" s="10" t="s">
-        <v>208</v>
-      </c>
       <c r="C51" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>0</v>
@@ -2652,10 +2654,10 @@
       <c r="H51" s="10"/>
       <c r="I51" s="10"/>
       <c r="J51" s="10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="K51" s="10" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="L51" s="9"/>
     </row>

</xml_diff>

<commit_message>
WAT API new test cases
</commit_message>
<xml_diff>
--- a/src/test/test-data/WATTestData.xlsx
+++ b/src/test/test-data/WATTestData.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="WoS_AuthorTransformation" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="224">
   <si>
     <t>GET</t>
   </si>
@@ -674,6 +674,46 @@
   </si>
   <si>
     <t>hits[0].totalTimesCited||hits[0].hIndex</t>
+  </si>
+  <si>
+    <t>WAT-807</t>
+  </si>
+  <si>
+    <t>Verify that Search Author API should return 400 if there is no "name" query param</t>
+  </si>
+  <si>
+    <t>status=400||error=Required query param 'name' is missing.</t>
+  </si>
+  <si>
+    <t>WAT-805</t>
+  </si>
+  <si>
+    <t>WAT-806</t>
+  </si>
+  <si>
+    <t>Verify that Search Author API should return 400 if there is empty name in query param</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?&amp;offset=0&amp;limit=10
+</t>
+  </si>
+  <si>
+    <t>?name=&amp;offset=0&amp;limit=10</t>
+  </si>
+  <si>
+    <t>status=400||error="A query param 'name' is empty.</t>
+  </si>
+  <si>
+    <t>Verify that Search Author API should return results if there is atleast one non-blank "name" query param and ignore any "name" query parameter that is empty</t>
+  </si>
+  <si>
+    <t>?name=upadhyaya&amp;offset=0&amp;limit=10&amp;name=</t>
+  </si>
+  <si>
+    <t>status=200||hits.primaryName=upadhyaya</t>
+  </si>
+  <si>
+    <t>hits[0].authorClusterId||hits[0].primaryName||hits[0].alternativeName||hits[0].organization||hits[0].department||hits[0].location||hits[0].totalNumberOfPublications||hits[0].publicationYearRangeMin||hits[0].publicationYearRangeMax||hits[0].topPublications</t>
   </si>
 </sst>
 </file>
@@ -1121,10 +1161,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E30" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2661,6 +2701,92 @@
       </c>
       <c r="L51" s="9"/>
     </row>
+    <row r="52" spans="1:12" ht="30">
+      <c r="A52" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F52" s="10"/>
+      <c r="G52" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="H52" s="10"/>
+      <c r="I52" s="10"/>
+      <c r="J52" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="K52" s="9"/>
+      <c r="L52" s="9"/>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="H53" s="10"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="K53" s="9"/>
+      <c r="L53" s="9"/>
+    </row>
+    <row r="54" spans="1:12" ht="105">
+      <c r="A54" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F54" s="10"/>
+      <c r="G54" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="H54" s="10"/>
+      <c r="I54" s="10"/>
+      <c r="J54" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="K54" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="L54" s="9"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A36" r:id="rId1" display="http://ent.jira.int.thomsonreuters.com/browse/WAT-535"/>

</xml_diff>

<commit_message>
WAT new API test cases
</commit_message>
<xml_diff>
--- a/src/test/test-data/WATTestData.xlsx
+++ b/src/test/test-data/WATTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="243">
   <si>
     <t>GET</t>
   </si>
@@ -720,6 +720,57 @@
   </si>
   <si>
     <t>hits[0].authorClusterId||hits[0].primaryName||hits[0].alternativeName||hits[0].department||hits[0].organization||hits[0].location||hits[0].totalNumberOfPublications||hits[0].publicationYearRangeMin||hits[0].publicationYearRangeMax||hits[0].topPublications</t>
+  </si>
+  <si>
+    <t>WAT-821</t>
+  </si>
+  <si>
+    <t>Verify that user is able to combine two or more authors using valid author id's</t>
+  </si>
+  <si>
+    <t>/author/combine</t>
+  </si>
+  <si>
+    <t>?authorId=20607616&amp;authorId=12678859</t>
+  </si>
+  <si>
+    <t>status=200||authorIds=20607616||authorIds=12678859</t>
+  </si>
+  <si>
+    <t>firstName||lastName||alternativeName||location||primaryAffiliation||department||affiliations||journals||totalTimesCited||hIndex</t>
+  </si>
+  <si>
+    <t>Verify that user is able to combine two or more authors using invalid author id's</t>
+  </si>
+  <si>
+    <t>WAT-822</t>
+  </si>
+  <si>
+    <t>WAT-823</t>
+  </si>
+  <si>
+    <t>WAT-824</t>
+  </si>
+  <si>
+    <t>status=200||authorIds=0||authorIds=0</t>
+  </si>
+  <si>
+    <t>Verify that user is able to combine two or more authors using missing author id's</t>
+  </si>
+  <si>
+    <t>?authorId=abc80451360&amp;authorId=def80451380</t>
+  </si>
+  <si>
+    <t>?authorId=&amp;authorId=</t>
+  </si>
+  <si>
+    <t>status=200||authorIds=0</t>
+  </si>
+  <si>
+    <t>Verify that combine API should not allow to combine only one author</t>
+  </si>
+  <si>
+    <t>?authorId=12678859</t>
   </si>
 </sst>
 </file>
@@ -1167,10 +1218,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L54"/>
+  <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2793,6 +2844,120 @@
       </c>
       <c r="L54" s="9"/>
     </row>
+    <row r="55" spans="1:12" ht="60">
+      <c r="A55" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F55" s="10"/>
+      <c r="G55" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="H55" s="10"/>
+      <c r="I55" s="10"/>
+      <c r="J55" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="K55" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="L55" s="9"/>
+    </row>
+    <row r="56" spans="1:12">
+      <c r="A56" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F56" s="10"/>
+      <c r="G56" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="H56" s="10"/>
+      <c r="I56" s="10"/>
+      <c r="J56" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="K56" s="9"/>
+      <c r="L56" s="9"/>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F57" s="10"/>
+      <c r="G57" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="H57" s="10"/>
+      <c r="I57" s="10"/>
+      <c r="J57" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="K57" s="9"/>
+      <c r="L57" s="9"/>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F58" s="10"/>
+      <c r="G58" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="H58" s="10"/>
+      <c r="I58" s="10"/>
+      <c r="J58" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="K58" s="9"/>
+      <c r="L58" s="9"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A36" r:id="rId1" display="http://ent.jira.int.thomsonreuters.com/browse/WAT-535"/>

</xml_diff>

<commit_message>
WAT new test cases
</commit_message>
<xml_diff>
--- a/src/test/test-data/WATTestData.xlsx
+++ b/src/test/test-data/WATTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="274">
   <si>
     <t>GET</t>
   </si>
@@ -813,6 +813,57 @@
   </si>
   <si>
     <t>status=200||authorIds=20607616||authorIds=12678859||authorIds=12614667</t>
+  </si>
+  <si>
+    <t>WAT-928</t>
+  </si>
+  <si>
+    <t>Verify that publication recommendations display on author record using authorId</t>
+  </si>
+  <si>
+    <t>/author/recommend/publications</t>
+  </si>
+  <si>
+    <t>?authorId=7781649</t>
+  </si>
+  <si>
+    <t>hits[0].authorId||hits[0].ut||hits[0].title||hits[0].authors||hits[0].journal||hits[0].volume||hits[0].issue||hits[0].published||hits[0].page||hits[0].timesCited||hits[0].score</t>
+  </si>
+  <si>
+    <t>Verify that max 3 publication recommendations display on author record</t>
+  </si>
+  <si>
+    <t>hits[0].authorId||hits[1].authorId||hits[2].authorId</t>
+  </si>
+  <si>
+    <t>WAT-929</t>
+  </si>
+  <si>
+    <t>Verify that publication recommendations display on author record using authorId and name</t>
+  </si>
+  <si>
+    <t>?authorId=7781649&amp;name=FABBRI, F.</t>
+  </si>
+  <si>
+    <t>WAT-930</t>
+  </si>
+  <si>
+    <t>WAT-931</t>
+  </si>
+  <si>
+    <t>WAT-932</t>
+  </si>
+  <si>
+    <t>Verify that publication recommendations should not display for missing authorId</t>
+  </si>
+  <si>
+    <t>?name=FABBRI, F.</t>
+  </si>
+  <si>
+    <t>Verify that each publication recommendations should have score</t>
+  </si>
+  <si>
+    <t>hits[0].score||hits[1].score||hits[2].score</t>
   </si>
 </sst>
 </file>
@@ -854,7 +905,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -903,11 +954,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -966,6 +1041,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1260,10 +1343,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L62"/>
+  <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E52" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L61" sqref="L61"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J70" sqref="J70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3091,34 +3174,182 @@
       <c r="L61" s="9"/>
     </row>
     <row r="62" spans="1:12" ht="30">
-      <c r="A62" s="9" t="s">
+      <c r="A62" s="16" t="s">
         <v>253</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="C62" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="D62" s="7" t="s">
+      <c r="C62" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="D62" s="12" t="s">
         <v>228</v>
       </c>
-      <c r="E62" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F62" s="10"/>
-      <c r="G62" s="10" t="s">
+      <c r="E62" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15" t="s">
         <v>245</v>
       </c>
-      <c r="H62" s="10"/>
-      <c r="I62" s="10"/>
-      <c r="J62" s="10" t="s">
+      <c r="H62" s="15"/>
+      <c r="I62" s="15"/>
+      <c r="J62" s="15" t="s">
         <v>256</v>
       </c>
-      <c r="K62" s="10" t="s">
+      <c r="K62" s="25" t="s">
         <v>255</v>
       </c>
       <c r="L62" s="9"/>
+    </row>
+    <row r="63" spans="1:12" ht="75">
+      <c r="A63" s="24" t="s">
+        <v>257</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F63" s="10"/>
+      <c r="G63" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="H63" s="10"/>
+      <c r="I63" s="10"/>
+      <c r="J63" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="K63" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="L63" s="9"/>
+    </row>
+    <row r="64" spans="1:12" ht="30">
+      <c r="A64" s="24" t="s">
+        <v>264</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F64" s="10"/>
+      <c r="G64" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="H64" s="10"/>
+      <c r="I64" s="10"/>
+      <c r="J64" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="L64" s="9"/>
+    </row>
+    <row r="65" spans="1:12" ht="75">
+      <c r="A65" s="24" t="s">
+        <v>267</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F65" s="10"/>
+      <c r="G65" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="H65" s="10"/>
+      <c r="I65" s="10"/>
+      <c r="J65" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="K65" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="L65" s="9"/>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F66" s="10"/>
+      <c r="G66" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="H66" s="10"/>
+      <c r="I66" s="10"/>
+      <c r="J66" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="K66" s="9"/>
+      <c r="L66" s="9"/>
+    </row>
+    <row r="67" spans="1:12" ht="30">
+      <c r="A67" s="27" t="s">
+        <v>269</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F67" s="10"/>
+      <c r="G67" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="H67" s="10"/>
+      <c r="I67" s="10"/>
+      <c r="J67" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="K67" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="L67" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
WAT Regression Script fixes
</commit_message>
<xml_diff>
--- a/src/test/test-data/WATTestData.xlsx
+++ b/src/test/test-data/WATTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="276">
   <si>
     <t>GET</t>
   </si>
@@ -102,9 +102,6 @@
     <t>status=200||info.limit=3</t>
   </si>
   <si>
-    <t>?authorId=1000469070&amp;sort=sortdate&amp;order=desc&amp;limit=3</t>
-  </si>
-  <si>
     <t>Verify that user is able to search for author cluster using only Last name</t>
   </si>
   <si>
@@ -216,28 +213,6 @@
     <t>?journal=physical</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Verify that given author id must associate with following fields
-authorClusterId,         
-utid,
-title,
-author,
-source,
-volume,
-issue,
-published, 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>page
-timesCited</t>
-    </r>
-  </si>
-  <si>
     <t>hits[0].authorClusterId||hits[0].primaryName||hits[0].alternativeNames||hits[0].affiliation||hits[0].location||hits[0].totalNumberOfPublications||hits[0].publicationYearRangeMin||hits[0].publicationYearRangeMax||hits[0].topPublications</t>
   </si>
   <si>
@@ -259,9 +234,6 @@
     <t>?authorId=20687704</t>
   </si>
   <si>
-    <t>status=200||hits.clusterId=20687704</t>
-  </si>
-  <si>
     <t>WAT-391</t>
   </si>
   <si>
@@ -286,15 +258,9 @@
     <t>status=200||info.limit=40||info.offset=20</t>
   </si>
   <si>
-    <t>hits[0].clusterId||hits[0].utid||hits[0].title||hits[0].authors||hits[0].source||hits[0].volume||hits[0].issue||hits[0].published||hits[0].page</t>
-  </si>
-  <si>
     <t>WAT-396</t>
   </si>
   <si>
-    <t>hits[0].clusterId||hits[1].clusterId||hits[2].clusterId</t>
-  </si>
-  <si>
     <t>WAT-397</t>
   </si>
   <si>
@@ -364,9 +330,6 @@
     <t>Verify that user is able to search author cluster when ORCID/RID is missing in the request</t>
   </si>
   <si>
-    <t>status=200||hits.authorClusterId=80453160</t>
-  </si>
-  <si>
     <t>Verify that user is able to search author cluster using invalid ORCID</t>
   </si>
   <si>
@@ -398,12 +361,6 @@
   </si>
   <si>
     <t>Verify that Author metadata should contain following fields, authorId. firstName, lastName, alternativeName, rid, location, primaryAffiliation, department, affiliations, totalTimesCited, hIndex</t>
-  </si>
-  <si>
-    <t>status=200||authorId=24303705||orcid=0000-0002-6423-7213</t>
-  </si>
-  <si>
-    <t>status=200||authorId=80453160||rid=A-9832-2009</t>
   </si>
   <si>
     <t>authorId=80453160||firstName=J M||lastName=TRANQUADA||alternativeName=TRANQUADA, JOHN||orcid=0000-0002-6423-7213||location=UPTON, NY, USA||primaryAffiliation=BROOKHAVEN NATL LAB||department=CONDENSED MATTER PHYS &amp; MAT SCI DEPT||affiliations=BROOKHAVEN NATL LABS||totalTimesCited=9165||hIndex=50</t>
@@ -692,9 +649,6 @@
     <t>?authorId=24549858&amp;authorId=20687704</t>
   </si>
   <si>
-    <t>status=200||hits.clusterId=24549858||hits.clusterId=20687704</t>
-  </si>
-  <si>
     <t>status=200||hits.primaryName=SMITH||hits.alternativeName=SMITH</t>
   </si>
   <si>
@@ -713,9 +667,6 @@
     <t>status=400</t>
   </si>
   <si>
-    <t>status=200||hits[0].clusterId=20687704</t>
-  </si>
-  <si>
     <t>status=200||hits.authorClusterId=7781649</t>
   </si>
   <si>
@@ -864,13 +815,59 @@
   </si>
   <si>
     <t>hits[0].score||hits[1].score||hits[2].score</t>
+  </si>
+  <si>
+    <t>DEPFAIL</t>
+  </si>
+  <si>
+    <t>status=200||hits.authorId=20687704</t>
+  </si>
+  <si>
+    <t>status=200||hits.authorId=24549858||hits.authorId=20687704</t>
+  </si>
+  <si>
+    <t>Verify that given author id must associate with following fields 
+authorId, 
+ut, 
+title, 
+authors, 
+journal, 
+volume, 
+issue, 
+published, 
+page and 
+timesCited</t>
+  </si>
+  <si>
+    <t>hits[0].authorId||hits[0].ut||hits[0].title||hits[0].authors||hits[0].journal||hits[0].volume||hits[0].issue||hits[0].published||hits[0].page||hits[0].timesCited</t>
+  </si>
+  <si>
+    <t>?authorId=20607616&amp;sort=year&amp;order=desc&amp;limit=3</t>
+  </si>
+  <si>
+    <t>status=200||hits[0].authorId=20687704</t>
+  </si>
+  <si>
+    <t>status=200||hits.authorClusterId=14990959</t>
+  </si>
+  <si>
+    <t>/author/(WAT-408_hits[0].authorClusterId)</t>
+  </si>
+  <si>
+    <t>status=200||authorId=(WAT-408_hits[0].authorClusterId)||orcid=0000-0002-6423-7213</t>
+  </si>
+  <si>
+    <t>/author/(WAT-504_hits[0].authorClusterId)</t>
+  </si>
+  <si>
+    <t>status=200||authorId=(WAT-504_hits[0].authorClusterId)||rid=A-9832-2009</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -885,10 +882,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1345,8 +1338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J70" sqref="J70"/>
+    <sheetView tabSelected="1" topLeftCell="E31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1405,138 +1398,138 @@
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" ht="135">
       <c r="A2" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="7" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
       <c r="J2" s="14" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="4" customFormat="1">
       <c r="A3" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>69</v>
-      </c>
       <c r="C3" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="10"/>
       <c r="G3" s="8" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
       <c r="J3" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K3" s="9"/>
       <c r="L3" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>70</v>
-      </c>
       <c r="C4" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="J4" s="7" t="s">
-        <v>72</v>
+        <v>265</v>
       </c>
       <c r="K4" s="9"/>
       <c r="L4" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="8" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="8" t="s">
-        <v>216</v>
+        <v>266</v>
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>0</v>
@@ -1552,53 +1545,53 @@
       </c>
       <c r="K6" s="16"/>
       <c r="L6" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>0</v>
@@ -1614,21 +1607,21 @@
       </c>
       <c r="K8" s="9"/>
       <c r="L8" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>0</v>
@@ -1644,60 +1637,60 @@
       </c>
       <c r="K9" s="9"/>
       <c r="L9" s="9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="164.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="165">
       <c r="A10" s="11" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>64</v>
+        <v>267</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="15"/>
       <c r="J10" s="14" t="s">
-        <v>223</v>
+        <v>270</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>81</v>
+        <v>268</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30">
       <c r="A11" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="7" t="s">
-        <v>26</v>
+        <v>269</v>
       </c>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
@@ -1705,472 +1698,474 @@
         <v>25</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="L11" s="9"/>
+        <v>253</v>
+      </c>
+      <c r="L11" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E12" s="21" t="s">
         <v>0</v>
       </c>
       <c r="F12" s="22"/>
       <c r="G12" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H12" s="22"/>
       <c r="I12" s="22"/>
       <c r="J12" s="23" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="K12" s="18"/>
       <c r="L12" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="6" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K13" s="9"/>
       <c r="L13" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" s="6" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="9" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
       <c r="J14" s="7" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="K14" s="9"/>
       <c r="L14" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="6" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
       <c r="J15" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K15" s="9"/>
       <c r="L15" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="9" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="7" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="K16" s="9"/>
       <c r="L16" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
       <c r="J17" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K17" s="16"/>
       <c r="L17" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
       <c r="J18" s="10" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="K18" s="9"/>
       <c r="L18" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
       <c r="J19" s="10" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="K19" s="9"/>
       <c r="L19" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
       <c r="J20" s="10" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="K20" s="9"/>
       <c r="L20" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F21" s="10"/>
       <c r="G21" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
       <c r="J21" s="10" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="K21" s="9"/>
       <c r="L21" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="6" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
       <c r="J22" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K22" s="9"/>
       <c r="L22" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
       <c r="J23" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K23" s="9"/>
       <c r="L23" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="30">
       <c r="A24" s="6" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
       <c r="J24" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K24" s="9"/>
       <c r="L24" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="30">
       <c r="A25" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="10"/>
       <c r="J25" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K25" s="9"/>
       <c r="L25" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="30">
       <c r="A26" s="6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F26" s="10"/>
       <c r="G26" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
       <c r="J26" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K26" s="9"/>
       <c r="L26" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="6" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>0</v>
@@ -2180,55 +2175,55 @@
       <c r="H27" s="10"/>
       <c r="I27" s="10"/>
       <c r="J27" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K27" s="9"/>
       <c r="L27" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="30">
       <c r="A28" s="6" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F28" s="15"/>
       <c r="G28" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H28" s="15"/>
       <c r="I28" s="15"/>
       <c r="J28" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K28" s="16"/>
       <c r="L28" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="105">
       <c r="A29" s="6" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>0</v>
@@ -2238,27 +2233,27 @@
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
       <c r="J29" s="10" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="L29" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="105">
       <c r="A30" s="6" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>0</v>
@@ -2268,27 +2263,27 @@
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
       <c r="J30" s="10" t="s">
-        <v>107</v>
+        <v>271</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L30" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="6" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C31" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D31" s="8" t="s">
         <v>157</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>165</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>0</v>
@@ -2298,25 +2293,25 @@
       <c r="H31" s="10"/>
       <c r="I31" s="10"/>
       <c r="J31" s="10" t="s">
-        <v>20</v>
+        <v>193</v>
       </c>
       <c r="K31" s="9"/>
       <c r="L31" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="6" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>0</v>
@@ -2330,21 +2325,21 @@
       </c>
       <c r="K32" s="9"/>
       <c r="L32" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="6" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>0</v>
@@ -2358,21 +2353,21 @@
       </c>
       <c r="K33" s="9"/>
       <c r="L33" s="9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="30">
       <c r="A34" s="9" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>170</v>
+        <v>272</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>0</v>
@@ -2380,29 +2375,31 @@
       <c r="F34" s="10"/>
       <c r="G34" s="9"/>
       <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
+      <c r="I34" s="10" t="s">
+        <v>104</v>
+      </c>
       <c r="J34" s="10" t="s">
-        <v>119</v>
+        <v>273</v>
       </c>
       <c r="K34" s="9" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="L34" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="9" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>0</v>
@@ -2412,25 +2409,25 @@
       <c r="H35" s="10"/>
       <c r="I35" s="10"/>
       <c r="J35" s="10" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="K35" s="9"/>
       <c r="L35" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="11" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>169</v>
+        <v>274</v>
       </c>
       <c r="E36" s="11" t="s">
         <v>0</v>
@@ -2438,27 +2435,29 @@
       <c r="F36" s="15"/>
       <c r="G36" s="16"/>
       <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
+      <c r="I36" s="15" t="s">
+        <v>106</v>
+      </c>
       <c r="J36" s="15" t="s">
-        <v>120</v>
+        <v>275</v>
       </c>
       <c r="K36" s="16"/>
       <c r="L36" s="9" t="s">
-        <v>126</v>
+        <v>264</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="180">
       <c r="A37" s="8" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>0</v>
@@ -2468,25 +2467,25 @@
       <c r="H37" s="10"/>
       <c r="I37" s="10"/>
       <c r="J37" s="7" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="K37" s="10" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="L37" s="9"/>
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="8" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>0</v>
@@ -2496,25 +2495,25 @@
       <c r="H38" s="10"/>
       <c r="I38" s="10"/>
       <c r="J38" s="10" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="K38" s="9"/>
       <c r="L38" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="9" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>0</v>
@@ -2524,27 +2523,27 @@
       <c r="H39" s="10"/>
       <c r="I39" s="10"/>
       <c r="J39" s="10" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="K39" s="9" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="L39" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="30">
       <c r="A40" s="9" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>0</v>
@@ -2554,87 +2553,87 @@
       <c r="H40" s="10"/>
       <c r="I40" s="10"/>
       <c r="J40" s="10" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="K40" s="9" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="L40" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="30">
       <c r="A41" s="16" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="E41" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F41" s="15"/>
       <c r="G41" s="15" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="H41" s="15"/>
       <c r="I41" s="15"/>
       <c r="J41" s="15" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="K41" s="16"/>
       <c r="L41" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="30">
       <c r="A42" s="9" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F42" s="10"/>
       <c r="G42" s="10" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="H42" s="10"/>
       <c r="I42" s="10"/>
       <c r="J42" s="10" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="K42" s="9"/>
       <c r="L42" s="9" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="30">
       <c r="A43" s="16" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="E43" s="16" t="s">
         <v>0</v>
@@ -2643,713 +2642,741 @@
       <c r="G43" s="16"/>
       <c r="H43" s="15"/>
       <c r="I43" s="11" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="J43" s="15" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="K43" s="16"/>
       <c r="L43" s="16" t="s">
-        <v>126</v>
+        <v>264</v>
       </c>
     </row>
     <row r="44" spans="1:12">
       <c r="A44" s="9" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F44" s="10"/>
       <c r="G44" s="10" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="H44" s="10"/>
       <c r="I44" s="10"/>
       <c r="J44" s="10" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="K44" s="10"/>
       <c r="L44" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="30">
       <c r="A45" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D45" s="7" t="s">
         <v>156</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>164</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F45" s="10"/>
       <c r="G45" s="10" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="H45" s="10"/>
       <c r="I45" s="10"/>
       <c r="J45" s="10" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="K45" s="9"/>
       <c r="L45" s="9"/>
     </row>
     <row r="46" spans="1:12" ht="45">
       <c r="A46" s="9" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F46" s="10"/>
       <c r="G46" s="10" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="H46" s="10"/>
       <c r="I46" s="10"/>
       <c r="J46" s="10" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="K46" s="9"/>
       <c r="L46" s="9"/>
     </row>
     <row r="47" spans="1:12">
       <c r="A47" s="9" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F47" s="10"/>
       <c r="G47" s="10" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="H47" s="10"/>
       <c r="I47" s="10"/>
       <c r="J47" s="10" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="K47" s="9"/>
       <c r="L47" s="9"/>
     </row>
     <row r="48" spans="1:12">
       <c r="A48" s="9" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F48" s="10"/>
       <c r="G48" s="10" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="H48" s="10"/>
       <c r="I48" s="10"/>
       <c r="J48" s="10" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="K48" s="9"/>
       <c r="L48" s="9"/>
     </row>
     <row r="49" spans="1:12" ht="30">
       <c r="A49" s="9" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F49" s="10"/>
       <c r="G49" s="10" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="H49" s="10"/>
       <c r="I49" s="10"/>
       <c r="J49" s="10" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="K49" s="9"/>
       <c r="L49" s="9"/>
     </row>
     <row r="50" spans="1:12" ht="45">
       <c r="A50" s="9" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F50" s="10"/>
       <c r="G50" s="10" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="H50" s="10"/>
       <c r="I50" s="10"/>
       <c r="J50" s="10" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="K50" s="10" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="L50" s="9"/>
     </row>
     <row r="51" spans="1:12" ht="60">
       <c r="A51" s="9" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F51" s="10"/>
       <c r="G51" s="10" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="H51" s="10"/>
       <c r="I51" s="10"/>
       <c r="J51" s="10" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="K51" s="10" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="L51" s="9"/>
     </row>
     <row r="52" spans="1:12" ht="30">
       <c r="A52" s="9" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F52" s="10"/>
       <c r="G52" s="10" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="H52" s="10"/>
       <c r="I52" s="10"/>
       <c r="J52" s="10" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="K52" s="9"/>
       <c r="L52" s="9"/>
     </row>
     <row r="53" spans="1:12">
       <c r="A53" s="9" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F53" s="10"/>
       <c r="G53" s="10" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="H53" s="10"/>
       <c r="I53" s="10"/>
       <c r="J53" s="10" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="K53" s="9"/>
-      <c r="L53" s="9"/>
+      <c r="L53" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="54" spans="1:12" ht="105">
       <c r="A54" s="9" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F54" s="10"/>
       <c r="G54" s="10" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="H54" s="10"/>
       <c r="I54" s="10"/>
       <c r="J54" s="10" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="K54" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="L54" s="9"/>
+        <v>201</v>
+      </c>
+      <c r="L54" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="55" spans="1:12" ht="60">
       <c r="A55" s="9" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F55" s="10"/>
       <c r="G55" s="10" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="H55" s="10"/>
       <c r="I55" s="10"/>
       <c r="J55" s="10" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="K55" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="L55" s="9"/>
+        <v>221</v>
+      </c>
+      <c r="L55" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="56" spans="1:12">
       <c r="A56" s="9" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F56" s="10"/>
       <c r="G56" s="10" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="H56" s="10"/>
       <c r="I56" s="10"/>
       <c r="J56" s="10" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="K56" s="9"/>
-      <c r="L56" s="9"/>
+      <c r="L56" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="9" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F57" s="10"/>
       <c r="G57" s="10" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="H57" s="10"/>
       <c r="I57" s="10"/>
       <c r="J57" s="10" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="K57" s="9"/>
-      <c r="L57" s="9"/>
+      <c r="L57" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="9" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F58" s="10"/>
       <c r="G58" s="10" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="H58" s="10"/>
       <c r="I58" s="10"/>
       <c r="J58" s="10" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="K58" s="9"/>
-      <c r="L58" s="9"/>
+      <c r="L58" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="59" spans="1:12" ht="60">
       <c r="A59" s="9" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="E59" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F59" s="10"/>
       <c r="G59" s="10" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="H59" s="10"/>
       <c r="I59" s="10"/>
       <c r="J59" s="10" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="K59" s="10" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="L59" s="9"/>
     </row>
     <row r="60" spans="1:12" ht="30">
       <c r="A60" s="9" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F60" s="10"/>
       <c r="G60" s="10" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="H60" s="10"/>
       <c r="I60" s="10"/>
       <c r="J60" s="10" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="K60" s="10" t="s">
-        <v>248</v>
-      </c>
-      <c r="L60" s="9"/>
+        <v>238</v>
+      </c>
+      <c r="L60" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="61" spans="1:12" ht="30">
       <c r="A61" s="9" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F61" s="10"/>
       <c r="G61" s="10" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="H61" s="10"/>
       <c r="I61" s="10"/>
       <c r="J61" s="10" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="K61" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="L61" s="9"/>
+        <v>242</v>
+      </c>
+      <c r="L61" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="62" spans="1:12" ht="30">
       <c r="A62" s="16" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="E62" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F62" s="15"/>
       <c r="G62" s="15" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="H62" s="15"/>
       <c r="I62" s="15"/>
       <c r="J62" s="15" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="K62" s="25" t="s">
-        <v>255</v>
-      </c>
-      <c r="L62" s="9"/>
+        <v>245</v>
+      </c>
+      <c r="L62" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="63" spans="1:12" ht="75">
       <c r="A63" s="24" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="E63" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F63" s="10"/>
       <c r="G63" s="10" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="H63" s="10"/>
       <c r="I63" s="10"/>
       <c r="J63" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K63" s="26" t="s">
-        <v>261</v>
-      </c>
-      <c r="L63" s="9"/>
+        <v>251</v>
+      </c>
+      <c r="L63" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="64" spans="1:12" ht="30">
       <c r="A64" s="24" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="E64" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F64" s="10"/>
       <c r="G64" s="10" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="H64" s="10"/>
       <c r="I64" s="10"/>
       <c r="J64" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="L64" s="9"/>
+        <v>253</v>
+      </c>
+      <c r="L64" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="65" spans="1:12" ht="75">
       <c r="A65" s="24" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="E65" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F65" s="10"/>
       <c r="G65" s="10" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="H65" s="10"/>
       <c r="I65" s="10"/>
       <c r="J65" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K65" s="26" t="s">
-        <v>261</v>
-      </c>
-      <c r="L65" s="9"/>
+        <v>251</v>
+      </c>
+      <c r="L65" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="24" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F66" s="10"/>
       <c r="G66" s="10" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="H66" s="10"/>
       <c r="I66" s="10"/>
       <c r="J66" s="10" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="K66" s="9"/>
-      <c r="L66" s="9"/>
+      <c r="L66" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="67" spans="1:12" ht="30">
       <c r="A67" s="27" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F67" s="10"/>
       <c r="G67" s="10" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="H67" s="10"/>
       <c r="I67" s="10"/>
       <c r="J67" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K67" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="L67" s="9"/>
+        <v>263</v>
+      </c>
+      <c r="L67" t="s">
+        <v>118</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
WAT new API scripts
</commit_message>
<xml_diff>
--- a/src/test/test-data/WATTestData.xlsx
+++ b/src/test/test-data/WATTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="287">
   <si>
     <t>GET</t>
   </si>
@@ -640,9 +640,6 @@
     <t>status=200||hits.primaryName=Tranquada||hits.location=USA||hits.organization=BROOKHAVEN NATL LAB||hits.topPublications=physical</t>
   </si>
   <si>
-    <t>?authorId=24549858</t>
-  </si>
-  <si>
     <t>?authorId=24549858&amp;authorId=20687704</t>
   </si>
   <si>
@@ -815,9 +812,6 @@
   </si>
   <si>
     <t>DEPFAIL</t>
-  </si>
-  <si>
-    <t>status=200||hits.authorId=20687704</t>
   </si>
   <si>
     <t>status=200||hits.authorId=24549858||hits.authorId=20687704</t>
@@ -862,12 +856,50 @@
   <si>
     <t>status=200||authorId=(WAT-388_hits[0].authorClusterId)||rid=A-9832-2009</t>
   </si>
+  <si>
+    <t>WAT-1007</t>
+  </si>
+  <si>
+    <t>Verify that get publications for one author should contain authorPosition to the each response payload</t>
+  </si>
+  <si>
+    <t>WAT-1008</t>
+  </si>
+  <si>
+    <t>Verify that get publications for one or more authors should contain authorPosition to the each response payload</t>
+  </si>
+  <si>
+    <t>?authorId=14990959</t>
+  </si>
+  <si>
+    <t>?authorId=20607616</t>
+  </si>
+  <si>
+    <t>status=200||hits.authorId=20607616</t>
+  </si>
+  <si>
+    <t>hits[0].authorPosition||hits[0].authorId</t>
+  </si>
+  <si>
+    <t>?authorId=(WAT-389_hits[0].authorId)</t>
+  </si>
+  <si>
+    <t>?authorId=(WAT-390_hits[0].authorId)&amp;authorId=(WAT-389_hits[0].authorId)</t>
+  </si>
+  <si>
+    <t>status=200||hits.authorId=(WAT-389_hits[0].authorId)||hits.authorPosition=(WAT-389_hits[0].authorPosition)</t>
+  </si>
+  <si>
+    <t>WAT-390||WAT-389</t>
+  </si>
+  <si>
+    <t>status=200||hits.authorId=(WAT-389_hits[0].authorId)||hits.authorId=(WAT-390_hits[0].authorId)||hits.authorPosition=(WAT-389_hits[0].authorPosition)||hits.authorPosition=(WAT-390_hits[0].authorPosition)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -899,7 +931,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -972,6 +1004,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1042,7 +1085,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1337,26 +1380,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L67"/>
+  <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E36" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" topLeftCell="E59" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J69" sqref="J69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="25.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="90.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="80.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="50.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="14.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="19.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="76.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="36.42578125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="90.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="80.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="50.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="76" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="36.42578125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1447,14 +1490,16 @@
       </c>
       <c r="F3" s="10"/>
       <c r="G3" s="8" t="s">
-        <v>205</v>
+        <v>278</v>
       </c>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
       <c r="J3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="9"/>
+      <c r="K3" s="9" t="s">
+        <v>281</v>
+      </c>
       <c r="L3" s="9" t="s">
         <v>118</v>
       </c>
@@ -1477,14 +1522,16 @@
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="8" t="s">
-        <v>69</v>
+        <v>279</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="J4" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="K4" s="9"/>
+        <v>280</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>281</v>
+      </c>
       <c r="L4" s="9" t="s">
         <v>118</v>
       </c>
@@ -1507,12 +1554,12 @@
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="8" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="9" t="s">
@@ -1646,7 +1693,7 @@
         <v>78</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>148</v>
@@ -1664,10 +1711,10 @@
       <c r="H10" s="10"/>
       <c r="I10" s="15"/>
       <c r="J10" s="14" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="L10" s="9" t="s">
         <v>118</v>
@@ -1691,7 +1738,7 @@
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="7" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
@@ -1699,7 +1746,7 @@
         <v>25</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="L11" t="s">
         <v>118</v>
@@ -1728,7 +1775,7 @@
       <c r="H12" s="22"/>
       <c r="I12" s="22"/>
       <c r="J12" s="23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K12" s="18"/>
       <c r="L12" s="9" t="s">
@@ -1830,7 +1877,7 @@
         <v>86</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>148</v>
@@ -1843,12 +1890,12 @@
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K16" s="9"/>
       <c r="L16" s="9" t="s">
@@ -1890,7 +1937,7 @@
         <v>88</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>148</v>
@@ -1908,7 +1955,7 @@
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
       <c r="J18" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K18" s="9"/>
       <c r="L18" s="9" t="s">
@@ -1938,7 +1985,7 @@
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
       <c r="J19" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K19" s="9"/>
       <c r="L19" s="9" t="s">
@@ -1968,7 +2015,7 @@
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
       <c r="J20" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K20" s="9"/>
       <c r="L20" s="9" t="s">
@@ -1998,7 +2045,7 @@
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
       <c r="J21" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K21" s="9"/>
       <c r="L21" s="9" t="s">
@@ -2234,10 +2281,10 @@
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
       <c r="J29" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="K29" s="7" t="s">
         <v>213</v>
-      </c>
-      <c r="K29" s="7" t="s">
-        <v>214</v>
       </c>
       <c r="L29" s="9" t="s">
         <v>118</v>
@@ -2264,7 +2311,7 @@
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
       <c r="J30" s="10" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="K30" s="7" t="s">
         <v>63</v>
@@ -2368,7 +2415,7 @@
         <v>148</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>0</v>
@@ -2380,13 +2427,13 @@
         <v>104</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="K34" s="9" t="s">
         <v>137</v>
       </c>
       <c r="L34" s="9" t="s">
-        <v>118</v>
+        <v>262</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -2428,7 +2475,7 @@
         <v>148</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E36" s="11" t="s">
         <v>0</v>
@@ -2440,7 +2487,7 @@
         <v>64</v>
       </c>
       <c r="J36" s="15" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="K36" s="16"/>
       <c r="L36" s="9" t="s">
@@ -2486,7 +2533,7 @@
         <v>148</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>0</v>
@@ -2498,7 +2545,7 @@
         <v>64</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="K38" s="9"/>
       <c r="L38" s="9" t="s">
@@ -2652,7 +2699,7 @@
       </c>
       <c r="K43" s="16"/>
       <c r="L43" s="16" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -2977,31 +3024,31 @@
     </row>
     <row r="55" spans="1:12" ht="60">
       <c r="A55" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="B55" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="B55" s="10" t="s">
+      <c r="C55" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D55" s="7" t="s">
         <v>216</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>217</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F55" s="10"/>
       <c r="G55" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H55" s="10"/>
       <c r="I55" s="10"/>
       <c r="J55" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="K55" s="10" t="s">
         <v>219</v>
-      </c>
-      <c r="K55" s="10" t="s">
-        <v>220</v>
       </c>
       <c r="L55" t="s">
         <v>118</v>
@@ -3009,28 +3056,28 @@
     </row>
     <row r="56" spans="1:12">
       <c r="A56" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>148</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F56" s="10"/>
       <c r="G56" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H56" s="10"/>
       <c r="I56" s="10"/>
       <c r="J56" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K56" s="9"/>
       <c r="L56" t="s">
@@ -3039,28 +3086,28 @@
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>148</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F57" s="10"/>
       <c r="G57" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H57" s="10"/>
       <c r="I57" s="10"/>
       <c r="J57" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K57" s="9"/>
       <c r="L57" t="s">
@@ -3069,28 +3116,28 @@
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C58" s="8" t="s">
         <v>148</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F58" s="10"/>
       <c r="G58" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H58" s="10"/>
       <c r="I58" s="10"/>
       <c r="J58" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K58" s="9"/>
       <c r="L58" t="s">
@@ -3099,61 +3146,61 @@
     </row>
     <row r="59" spans="1:12" ht="60">
       <c r="A59" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="B59" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="B59" s="10" t="s">
-        <v>233</v>
-      </c>
       <c r="C59" s="8" t="s">
         <v>148</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E59" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F59" s="10"/>
       <c r="G59" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H59" s="10"/>
       <c r="I59" s="10"/>
       <c r="J59" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="K59" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="L59" s="9"/>
     </row>
     <row r="60" spans="1:12" ht="30">
       <c r="A60" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C60" s="8" t="s">
         <v>148</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F60" s="10"/>
       <c r="G60" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H60" s="10"/>
       <c r="I60" s="10"/>
       <c r="J60" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K60" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L60" t="s">
         <v>118</v>
@@ -3161,31 +3208,31 @@
     </row>
     <row r="61" spans="1:12" ht="30">
       <c r="A61" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C61" s="8" t="s">
         <v>148</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F61" s="10"/>
       <c r="G61" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H61" s="10"/>
       <c r="I61" s="10"/>
       <c r="J61" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K61" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L61" t="s">
         <v>118</v>
@@ -3193,31 +3240,31 @@
     </row>
     <row r="62" spans="1:12" ht="30">
       <c r="A62" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>243</v>
-      </c>
       <c r="C62" s="13" t="s">
         <v>148</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E62" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F62" s="15"/>
       <c r="G62" s="15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H62" s="15"/>
       <c r="I62" s="15"/>
       <c r="J62" s="15" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K62" s="25" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="L62" t="s">
         <v>118</v>
@@ -3225,23 +3272,23 @@
     </row>
     <row r="63" spans="1:12" ht="75">
       <c r="A63" s="24" t="s">
+        <v>245</v>
+      </c>
+      <c r="B63" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="B63" s="10" t="s">
+      <c r="C63" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D63" s="7" t="s">
         <v>247</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="D63" s="7" t="s">
-        <v>248</v>
       </c>
       <c r="E63" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F63" s="10"/>
       <c r="G63" s="10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H63" s="10"/>
       <c r="I63" s="10"/>
@@ -3249,7 +3296,7 @@
         <v>27</v>
       </c>
       <c r="K63" s="26" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="L63" t="s">
         <v>118</v>
@@ -3257,23 +3304,23 @@
     </row>
     <row r="64" spans="1:12" ht="30">
       <c r="A64" s="24" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C64" s="8" t="s">
         <v>148</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E64" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F64" s="10"/>
       <c r="G64" s="10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H64" s="10"/>
       <c r="I64" s="10"/>
@@ -3281,7 +3328,7 @@
         <v>27</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="L64" t="s">
         <v>118</v>
@@ -3289,23 +3336,23 @@
     </row>
     <row r="65" spans="1:12" ht="75">
       <c r="A65" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C65" s="8" t="s">
         <v>148</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E65" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F65" s="10"/>
       <c r="G65" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H65" s="10"/>
       <c r="I65" s="10"/>
@@ -3313,7 +3360,7 @@
         <v>27</v>
       </c>
       <c r="K65" s="26" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="L65" t="s">
         <v>118</v>
@@ -3321,28 +3368,28 @@
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="24" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C66" s="8" t="s">
         <v>148</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F66" s="10"/>
       <c r="G66" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H66" s="10"/>
       <c r="I66" s="10"/>
       <c r="J66" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K66" s="9"/>
       <c r="L66" t="s">
@@ -3351,33 +3398,97 @@
     </row>
     <row r="67" spans="1:12" ht="30">
       <c r="A67" s="27" t="s">
-        <v>258</v>
-      </c>
-      <c r="B67" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="B67" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="C67" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="E67" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F67" s="15"/>
+      <c r="G67" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="H67" s="15"/>
+      <c r="I67" s="15"/>
+      <c r="J67" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K67" s="15" t="s">
         <v>261</v>
       </c>
-      <c r="C67" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="D67" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F67" s="10"/>
-      <c r="G67" s="10" t="s">
-        <v>255</v>
-      </c>
-      <c r="H67" s="10"/>
-      <c r="I67" s="10"/>
-      <c r="J67" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="K67" s="10" t="s">
-        <v>262</v>
-      </c>
       <c r="L67" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="30">
+      <c r="A68" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="E68" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F68" s="10"/>
+      <c r="G68" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="H68" s="10"/>
+      <c r="I68" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="J68" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="K68" s="9"/>
+      <c r="L68" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="60">
+      <c r="A69" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D69" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F69" s="10"/>
+      <c r="G69" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="H69" s="10"/>
+      <c r="I69" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="J69" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="K69" s="9"/>
+      <c r="L69" t="s">
         <v>118</v>
       </c>
     </row>

</xml_diff>

<commit_message>
WAT API Regression script changes
</commit_message>
<xml_diff>
--- a/src/test/test-data/WATTestData.xlsx
+++ b/src/test/test-data/WATTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="285">
   <si>
     <t>GET</t>
   </si>
@@ -168,9 +168,6 @@
     <t>?name=SMITH,JOHN</t>
   </si>
   <si>
-    <t>status=200||hits.primaryName=SMITH, JOHN</t>
-  </si>
-  <si>
     <t>Verify that user is able to search for author cluster using  Last name and First Name with intials(complete name)</t>
   </si>
   <si>
@@ -274,9 +271,6 @@
   </si>
   <si>
     <t>?name=SMITH, JOHN H</t>
-  </si>
-  <si>
-    <t>status=200||hits.primaryName=SMITH, JOHN H</t>
   </si>
   <si>
     <t>WAT-401</t>
@@ -725,9 +719,6 @@
   </si>
   <si>
     <t>?authorId=20607616&amp;authorId=12678859&amp;authorId=12614667</t>
-  </si>
-  <si>
-    <t>status=200||authorIds=20607616||authorIds=12678859||authorId=12614667</t>
   </si>
   <si>
     <t>Verify that metrics(totalTimesCited,hIndex) should display after combine two or more author's</t>
@@ -894,6 +885,9 @@
   </si>
   <si>
     <t>status=200||hits.authorId=(WAT-389_hits[0].authorId)||hits.authorId=(WAT-390_hits[0].authorId)||hits.authorPosition=(WAT-389_hits[0].authorPosition)||hits.authorPosition=(WAT-390_hits[0].authorPosition)</t>
+  </si>
+  <si>
+    <t>status=200||hits.primaryName=SMITH</t>
   </si>
 </sst>
 </file>
@@ -1019,7 +1013,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1086,6 +1080,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1382,8 +1377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E59" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K69" sqref="K69"/>
+    <sheetView tabSelected="1" topLeftCell="E51" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J59" sqref="J59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1442,55 +1437,55 @@
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" ht="135">
       <c r="A2" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
       <c r="J2" s="14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="4" customFormat="1">
       <c r="A3" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="10"/>
       <c r="G3" s="8" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
@@ -1498,86 +1493,86 @@
         <v>27</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="8" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="J4" s="7" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="8" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>0</v>
@@ -1593,53 +1588,53 @@
       </c>
       <c r="K6" s="16"/>
       <c r="L6" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>0</v>
@@ -1655,21 +1650,21 @@
       </c>
       <c r="K8" s="9"/>
       <c r="L8" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>0</v>
@@ -1685,60 +1680,60 @@
       </c>
       <c r="K9" s="9"/>
       <c r="L9" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="165">
       <c r="A10" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="15"/>
       <c r="J10" s="14" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30">
       <c r="A11" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="7" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
@@ -1746,24 +1741,24 @@
         <v>25</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="L11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B12" s="20" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E12" s="21" t="s">
         <v>0</v>
@@ -1775,25 +1770,25 @@
       <c r="H12" s="22"/>
       <c r="I12" s="22"/>
       <c r="J12" s="23" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K12" s="18"/>
       <c r="L12" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>46</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>0</v>
@@ -1805,265 +1800,265 @@
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="7" t="s">
-        <v>48</v>
+        <v>284</v>
       </c>
       <c r="K13" s="9"/>
       <c r="L13" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
       <c r="J14" s="7" t="s">
-        <v>84</v>
+        <v>284</v>
       </c>
       <c r="K14" s="9"/>
       <c r="L14" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
       <c r="J15" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K15" s="9"/>
       <c r="L15" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="9" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="K16" s="9"/>
       <c r="L16" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
       <c r="J17" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K17" s="16"/>
       <c r="L17" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
       <c r="J18" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K18" s="9"/>
       <c r="L18" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
       <c r="J19" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K19" s="9"/>
       <c r="L19" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
       <c r="J20" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K20" s="9"/>
       <c r="L20" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F21" s="10"/>
       <c r="G21" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
       <c r="J21" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K21" s="9"/>
       <c r="L21" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>32</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>0</v>
@@ -2079,21 +2074,21 @@
       </c>
       <c r="K22" s="9"/>
       <c r="L22" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>33</v>
       </c>
       <c r="C23" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>148</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>150</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>0</v>
@@ -2109,21 +2104,21 @@
       </c>
       <c r="K23" s="9"/>
       <c r="L23" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="30">
       <c r="A24" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C24" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>148</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>150</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>0</v>
@@ -2139,21 +2134,21 @@
       </c>
       <c r="K24" s="9"/>
       <c r="L24" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="30">
       <c r="A25" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>35</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>0</v>
@@ -2169,21 +2164,21 @@
       </c>
       <c r="K25" s="9"/>
       <c r="L25" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="30">
       <c r="A26" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>36</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>0</v>
@@ -2199,21 +2194,21 @@
       </c>
       <c r="K26" s="9"/>
       <c r="L26" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>37</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>0</v>
@@ -2227,21 +2222,21 @@
       </c>
       <c r="K27" s="9"/>
       <c r="L27" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="30">
       <c r="A28" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>31</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>0</v>
@@ -2257,21 +2252,21 @@
       </c>
       <c r="K28" s="16"/>
       <c r="L28" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="105">
       <c r="A29" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>0</v>
@@ -2281,27 +2276,27 @@
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
       <c r="J29" s="10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="L29" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="105">
       <c r="A30" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>0</v>
@@ -2311,27 +2306,27 @@
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
       <c r="J30" s="10" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L30" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>0</v>
@@ -2341,25 +2336,25 @@
       <c r="H31" s="10"/>
       <c r="I31" s="10"/>
       <c r="J31" s="10" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="K31" s="9"/>
       <c r="L31" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>0</v>
@@ -2373,21 +2368,21 @@
       </c>
       <c r="K32" s="9"/>
       <c r="L32" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>0</v>
@@ -2401,21 +2396,21 @@
       </c>
       <c r="K33" s="9"/>
       <c r="L33" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="30">
       <c r="A34" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>0</v>
@@ -2424,30 +2419,30 @@
       <c r="G34" s="9"/>
       <c r="H34" s="10"/>
       <c r="I34" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="K34" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L34" s="9" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>0</v>
@@ -2457,25 +2452,25 @@
       <c r="H35" s="10"/>
       <c r="I35" s="10"/>
       <c r="J35" s="10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="K35" s="9"/>
       <c r="L35" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E36" s="11" t="s">
         <v>0</v>
@@ -2484,28 +2479,28 @@
       <c r="G36" s="16"/>
       <c r="H36" s="15"/>
       <c r="I36" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J36" s="15" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="K36" s="16"/>
       <c r="L36" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="180">
       <c r="A37" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>0</v>
@@ -2515,25 +2510,25 @@
       <c r="H37" s="10"/>
       <c r="I37" s="10"/>
       <c r="J37" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K37" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="L37" s="9"/>
     </row>
     <row r="38" spans="1:12" ht="30">
       <c r="A38" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>0</v>
@@ -2542,28 +2537,28 @@
       <c r="G38" s="9"/>
       <c r="H38" s="10"/>
       <c r="I38" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="K38" s="9"/>
       <c r="L38" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>0</v>
@@ -2573,27 +2568,27 @@
       <c r="H39" s="10"/>
       <c r="I39" s="10"/>
       <c r="J39" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="K39" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L39" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="30">
       <c r="A40" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>0</v>
@@ -2603,87 +2598,87 @@
       <c r="H40" s="10"/>
       <c r="I40" s="10"/>
       <c r="J40" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K40" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="L40" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="30">
       <c r="A41" s="16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E41" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F41" s="15"/>
       <c r="G41" s="15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H41" s="15"/>
       <c r="I41" s="15"/>
       <c r="J41" s="15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="K41" s="16"/>
       <c r="L41" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="30">
       <c r="A42" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F42" s="10"/>
       <c r="G42" s="10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H42" s="10"/>
       <c r="I42" s="10"/>
       <c r="J42" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K42" s="9"/>
       <c r="L42" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="30">
       <c r="A43" s="16" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E43" s="16" t="s">
         <v>0</v>
@@ -2692,603 +2687,603 @@
       <c r="G43" s="16"/>
       <c r="H43" s="15"/>
       <c r="I43" s="11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J43" s="15" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K43" s="16"/>
       <c r="L43" s="16" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="44" spans="1:12">
       <c r="A44" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F44" s="10"/>
       <c r="G44" s="10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H44" s="10"/>
       <c r="I44" s="10"/>
       <c r="J44" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K44" s="10"/>
       <c r="L44" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="30">
       <c r="A45" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F45" s="10"/>
       <c r="G45" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H45" s="10"/>
       <c r="I45" s="10"/>
       <c r="J45" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="K45" s="9"/>
       <c r="L45" s="9"/>
     </row>
     <row r="46" spans="1:12" ht="45">
-      <c r="A46" s="9" t="s">
-        <v>164</v>
+      <c r="A46" s="28" t="s">
+        <v>162</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F46" s="10"/>
       <c r="G46" s="10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H46" s="10"/>
       <c r="I46" s="10"/>
       <c r="J46" s="10" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="K46" s="9"/>
       <c r="L46" s="9"/>
     </row>
     <row r="47" spans="1:12">
-      <c r="A47" s="9" t="s">
-        <v>168</v>
+      <c r="A47" s="28" t="s">
+        <v>166</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F47" s="10"/>
       <c r="G47" s="10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H47" s="10"/>
       <c r="I47" s="10"/>
       <c r="J47" s="10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K47" s="9"/>
       <c r="L47" s="9"/>
     </row>
     <row r="48" spans="1:12">
-      <c r="A48" s="9" t="s">
-        <v>175</v>
+      <c r="A48" s="28" t="s">
+        <v>173</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F48" s="10"/>
       <c r="G48" s="10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H48" s="10"/>
       <c r="I48" s="10"/>
       <c r="J48" s="10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K48" s="9"/>
       <c r="L48" s="9"/>
     </row>
     <row r="49" spans="1:12" ht="30">
-      <c r="A49" s="9" t="s">
-        <v>177</v>
+      <c r="A49" s="28" t="s">
+        <v>175</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F49" s="10"/>
       <c r="G49" s="10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H49" s="10"/>
       <c r="I49" s="10"/>
       <c r="J49" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="K49" s="9"/>
       <c r="L49" s="9"/>
     </row>
     <row r="50" spans="1:12" ht="45">
-      <c r="A50" s="9" t="s">
+      <c r="A50" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="B50" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="B50" s="10" t="s">
-        <v>184</v>
-      </c>
       <c r="C50" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F50" s="10"/>
       <c r="G50" s="10" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H50" s="10"/>
       <c r="I50" s="10"/>
       <c r="J50" s="10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K50" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="L50" s="9"/>
+    </row>
+    <row r="51" spans="1:12" ht="60">
+      <c r="A51" s="28" t="s">
         <v>181</v>
       </c>
-      <c r="L50" s="9"/>
-    </row>
-    <row r="51" spans="1:12" ht="60">
-      <c r="A51" s="9" t="s">
+      <c r="B51" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="B51" s="10" t="s">
-        <v>185</v>
-      </c>
       <c r="C51" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F51" s="10"/>
       <c r="G51" s="10" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H51" s="10"/>
       <c r="I51" s="10"/>
       <c r="J51" s="10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K51" s="10" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="L51" s="9"/>
     </row>
     <row r="52" spans="1:12" ht="30">
       <c r="A52" s="9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F52" s="10"/>
       <c r="G52" s="10" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H52" s="10"/>
       <c r="I52" s="10"/>
       <c r="J52" s="10" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="K52" s="9"/>
       <c r="L52" s="9"/>
     </row>
     <row r="53" spans="1:12">
       <c r="A53" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F53" s="10"/>
       <c r="G53" s="10" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H53" s="10"/>
       <c r="I53" s="10"/>
       <c r="J53" s="10" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K53" s="9"/>
       <c r="L53" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="105">
       <c r="A54" s="9" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F54" s="10"/>
       <c r="G54" s="10" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H54" s="10"/>
       <c r="I54" s="10"/>
       <c r="J54" s="10" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="K54" s="7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L54" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="60">
       <c r="A55" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D55" s="7" t="s">
         <v>214</v>
-      </c>
-      <c r="B55" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>216</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F55" s="10"/>
       <c r="G55" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H55" s="10"/>
       <c r="I55" s="10"/>
       <c r="J55" s="10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="K55" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="L55" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="56" spans="1:12">
       <c r="A56" s="9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F56" s="10"/>
       <c r="G56" s="10" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H56" s="10"/>
       <c r="I56" s="10"/>
       <c r="J56" s="10" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="K56" s="9"/>
       <c r="L56" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="9" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F57" s="10"/>
       <c r="G57" s="10" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H57" s="10"/>
       <c r="I57" s="10"/>
       <c r="J57" s="10" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="K57" s="9"/>
       <c r="L57" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="9" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F58" s="10"/>
       <c r="G58" s="10" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H58" s="10"/>
       <c r="I58" s="10"/>
       <c r="J58" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K58" s="9"/>
       <c r="L58" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="60">
       <c r="A59" s="9" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E59" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F59" s="10"/>
       <c r="G59" s="10" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H59" s="10"/>
       <c r="I59" s="10"/>
       <c r="J59" s="10" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="K59" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="L59" s="9"/>
     </row>
     <row r="60" spans="1:12" ht="30">
       <c r="A60" s="9" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F60" s="10"/>
       <c r="G60" s="10" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H60" s="10"/>
       <c r="I60" s="10"/>
       <c r="J60" s="10" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="K60" s="10" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="L60" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:12" ht="30">
       <c r="A61" s="9" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F61" s="10"/>
       <c r="G61" s="10" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H61" s="10"/>
       <c r="I61" s="10"/>
       <c r="J61" s="10" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="K61" s="10" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="L61" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="62" spans="1:12" ht="30">
       <c r="A62" s="16" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E62" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F62" s="15"/>
       <c r="G62" s="15" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H62" s="15"/>
       <c r="I62" s="15"/>
       <c r="J62" s="15" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="K62" s="25" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="L62" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="63" spans="1:12" ht="75">
       <c r="A63" s="24" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E63" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F63" s="10"/>
       <c r="G63" s="10" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="H63" s="10"/>
       <c r="I63" s="10"/>
@@ -3296,31 +3291,31 @@
         <v>27</v>
       </c>
       <c r="K63" s="26" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="L63" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="64" spans="1:12" ht="30">
       <c r="A64" s="24" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E64" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F64" s="10"/>
       <c r="G64" s="10" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="H64" s="10"/>
       <c r="I64" s="10"/>
@@ -3328,31 +3323,31 @@
         <v>27</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="L64" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="65" spans="1:12" ht="75">
       <c r="A65" s="24" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E65" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F65" s="10"/>
       <c r="G65" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="H65" s="10"/>
       <c r="I65" s="10"/>
@@ -3360,61 +3355,61 @@
         <v>27</v>
       </c>
       <c r="K65" s="26" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="L65" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="24" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F66" s="10"/>
       <c r="G66" s="10" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="H66" s="10"/>
       <c r="I66" s="10"/>
       <c r="J66" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K66" s="9"/>
       <c r="L66" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="67" spans="1:12" ht="30">
       <c r="A67" s="27" t="s">
+        <v>254</v>
+      </c>
+      <c r="B67" s="15" t="s">
         <v>257</v>
       </c>
-      <c r="B67" s="15" t="s">
-        <v>260</v>
-      </c>
       <c r="C67" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E67" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F67" s="15"/>
       <c r="G67" s="15" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="H67" s="15"/>
       <c r="I67" s="15"/>
@@ -3422,74 +3417,74 @@
         <v>27</v>
       </c>
       <c r="K67" s="15" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="L67" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="68" spans="1:12" ht="30">
       <c r="A68" s="9" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E68" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F68" s="10"/>
       <c r="G68" s="10" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="H68" s="10"/>
       <c r="I68" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J68" s="15" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="K68" s="9"/>
       <c r="L68" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="69" spans="1:12" ht="60">
       <c r="A69" s="9" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E69" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F69" s="10"/>
       <c r="G69" s="10" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="H69" s="10"/>
       <c r="I69" s="10" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J69" s="10" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="K69" s="9"/>
       <c r="L69" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WAT API script  changes
</commit_message>
<xml_diff>
--- a/src/test/test-data/WATTestData.xlsx
+++ b/src/test/test-data/WATTestData.xlsx
@@ -519,30 +519,12 @@
     <t>Verify that user should be able to filter values for an author using provided filter name,affiliation,category</t>
   </si>
   <si>
-    <t>?name=manalang&amp;country=USA&amp;affiliation=UNIV MISSOURI&amp;filter=name&amp;filter=affiliation&amp;filter=category</t>
-  </si>
-  <si>
-    <t>status=200||filters.primaryName=manalang||filters.category=PEDIATRICSHEMATOLOGY|||filters.affiliation=UNIV MISSOURI</t>
-  </si>
-  <si>
     <t>WAT-411</t>
   </si>
   <si>
-    <t>?name=manalang&amp;filter=name</t>
-  </si>
-  <si>
     <t>status=200||hits.primaryName=manalang||filters.primaryName=manalang</t>
   </si>
   <si>
-    <t>?name=bhavya&amp;affiliation=indian&amp;filter=affiliation</t>
-  </si>
-  <si>
-    <t>status=200||hits.primaryName=bhavya||filters.affiliation=indian</t>
-  </si>
-  <si>
-    <t>?name=bhavya&amp;category=AGRICULTURE&amp;filter=category</t>
-  </si>
-  <si>
     <t>status=200||hits.primaryName=bhavya||filters.category=AGRICULTURE</t>
   </si>
   <si>
@@ -561,9 +543,6 @@
     <t>Verify that user should be able to filter values for an author using 'affiliation' filter</t>
   </si>
   <si>
-    <t>status=200||hits.primaryName=wang||filters.category=physics||hits.affiliation=china</t>
-  </si>
-  <si>
     <t>hits[0].publicationYearRangeMin||hits.publicationYearRangeMax</t>
   </si>
   <si>
@@ -580,12 +559,6 @@
   </si>
   <si>
     <t>hits[0].totalNumberOfPublications</t>
-  </si>
-  <si>
-    <t>?name=wang&amp;affiliation=china&amp;filter=name&amp;category=physics&amp;filter=affiliation&amp;filter=category&amp;filters.category&amp;sort=year&amp;order=asc&amp;limit=10</t>
-  </si>
-  <si>
-    <t>?name=wang&amp;affiliation=china&amp;filter=name&amp;category=physics&amp;filter=affiliation&amp;filter=category&amp;filters.category&amp;sort=totalNumberOfPublications&amp;order=asc&amp;limit=10</t>
   </si>
   <si>
     <t>hits[0].totalTimesCited||hits[0].hIndex</t>
@@ -1122,6 +1095,33 @@
   </si>
   <si>
     <t>WAT-1114</t>
+  </si>
+  <si>
+    <t>?name=manalang&amp;fltr=name</t>
+  </si>
+  <si>
+    <t>?name=bhavya&amp;affiliation=indian&amp;fltr=org</t>
+  </si>
+  <si>
+    <t>?name=manalang&amp;country=USA&amp;affiliation=UNIV MISSOURI&amp;fltr=name&amp;fltr=org&amp;fltr=cat</t>
+  </si>
+  <si>
+    <t>?name=bhavya&amp;category=AGRICULTURE&amp;fltr=cat</t>
+  </si>
+  <si>
+    <t>?name=wang&amp;affiliation=china&amp;fltr=name&amp;category=physics&amp;fltr=org&amp;fltr=cat&amp;filters.category&amp;sort=year&amp;order=asc&amp;limit=10</t>
+  </si>
+  <si>
+    <t>?name=wang&amp;affiliation=china&amp;fltr=name&amp;category=physics&amp;fltr=org&amp;fltr=cat&amp;filters.category&amp;sort=totalNumberOfPublications&amp;order=asc&amp;limit=10</t>
+  </si>
+  <si>
+    <t>status=200||filters.primaryName=manalang||filters.category=PEDIATRICSHEMATOLOGY|||filters.organization=UNIV MISSOURI</t>
+  </si>
+  <si>
+    <t>status=200||hits.primaryName=bhavya||filters.organization=indian</t>
+  </si>
+  <si>
+    <t>status=200||hits.primaryName=wang||filters.category=physics||hits.organization=china</t>
   </si>
 </sst>
 </file>
@@ -1611,8 +1611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89"/>
+    <sheetView tabSelected="1" topLeftCell="C45" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1687,15 +1687,15 @@
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="7" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
       <c r="J2" s="14" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>116</v>
@@ -1719,7 +1719,7 @@
       </c>
       <c r="F3" s="10"/>
       <c r="G3" s="8" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
@@ -1727,7 +1727,7 @@
         <v>27</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="L3" s="9" t="s">
         <v>116</v>
@@ -1751,15 +1751,15 @@
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="8" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="J4" s="7" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="L4" s="9" t="s">
         <v>116</v>
@@ -1783,12 +1783,12 @@
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="8" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="8" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="9" t="s">
@@ -1922,7 +1922,7 @@
         <v>77</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>146</v>
@@ -1940,10 +1940,10 @@
       <c r="H10" s="10"/>
       <c r="I10" s="15"/>
       <c r="J10" s="14" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="L10" s="9" t="s">
         <v>116</v>
@@ -1967,7 +1967,7 @@
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="7" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
@@ -1975,7 +1975,7 @@
         <v>25</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="L11" t="s">
         <v>116</v>
@@ -2004,7 +2004,7 @@
       <c r="H12" s="22"/>
       <c r="I12" s="22"/>
       <c r="J12" s="23" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="K12" s="18"/>
       <c r="L12" s="9" t="s">
@@ -2034,7 +2034,7 @@
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="7" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="K13" s="9"/>
       <c r="L13" s="9" t="s">
@@ -2064,7 +2064,7 @@
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
       <c r="J14" s="7" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="K14" s="9"/>
       <c r="L14" s="9" t="s">
@@ -2106,7 +2106,7 @@
         <v>84</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>146</v>
@@ -2119,12 +2119,12 @@
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="9" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="7" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="K16" s="9"/>
       <c r="L16" s="9" t="s">
@@ -2166,7 +2166,7 @@
         <v>86</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>146</v>
@@ -2184,7 +2184,7 @@
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
       <c r="J18" s="10" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="K18" s="9"/>
       <c r="L18" s="9" t="s">
@@ -2214,7 +2214,7 @@
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
       <c r="J19" s="10" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="K19" s="9"/>
       <c r="L19" s="9" t="s">
@@ -2244,7 +2244,7 @@
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
       <c r="J20" s="10" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="K20" s="9"/>
       <c r="L20" s="9" t="s">
@@ -2274,7 +2274,7 @@
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
       <c r="J21" s="10" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="K21" s="9"/>
       <c r="L21" s="9" t="s">
@@ -2510,10 +2510,10 @@
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
       <c r="J29" s="10" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="L29" s="9" t="s">
         <v>116</v>
@@ -2540,7 +2540,7 @@
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
       <c r="J30" s="10" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="K30" s="7" t="s">
         <v>62</v>
@@ -2570,7 +2570,7 @@
       <c r="H31" s="10"/>
       <c r="I31" s="10"/>
       <c r="J31" s="10" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="K31" s="9"/>
       <c r="L31" s="9" t="s">
@@ -2644,7 +2644,7 @@
         <v>146</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>0</v>
@@ -2656,13 +2656,13 @@
         <v>102</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="K34" s="9" t="s">
         <v>135</v>
       </c>
       <c r="L34" s="9" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -2704,7 +2704,7 @@
         <v>146</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="E36" s="11" t="s">
         <v>0</v>
@@ -2716,11 +2716,11 @@
         <v>63</v>
       </c>
       <c r="J36" s="15" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="K36" s="16"/>
       <c r="L36" s="9" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="180">
@@ -2762,7 +2762,7 @@
         <v>146</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>0</v>
@@ -2774,11 +2774,11 @@
         <v>63</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="K38" s="9"/>
       <c r="L38" s="9" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -2835,7 +2835,7 @@
         <v>122</v>
       </c>
       <c r="K40" s="9" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="L40" s="9" t="s">
         <v>116</v>
@@ -2928,7 +2928,7 @@
       </c>
       <c r="K43" s="16"/>
       <c r="L43" s="16" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -2989,7 +2989,7 @@
       <c r="K45" s="9"/>
       <c r="L45" s="9"/>
     </row>
-    <row r="46" spans="1:12" ht="45">
+    <row r="46" spans="1:12" ht="30">
       <c r="A46" s="28" t="s">
         <v>162</v>
       </c>
@@ -3007,22 +3007,22 @@
       </c>
       <c r="F46" s="10"/>
       <c r="G46" s="10" t="s">
-        <v>164</v>
+        <v>355</v>
       </c>
       <c r="H46" s="10"/>
       <c r="I46" s="10"/>
       <c r="J46" s="10" t="s">
-        <v>165</v>
+        <v>359</v>
       </c>
       <c r="K46" s="9"/>
       <c r="L46" s="9"/>
     </row>
     <row r="47" spans="1:12">
       <c r="A47" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>146</v>
@@ -3035,22 +3035,22 @@
       </c>
       <c r="F47" s="10"/>
       <c r="G47" s="10" t="s">
-        <v>167</v>
+        <v>353</v>
       </c>
       <c r="H47" s="10"/>
       <c r="I47" s="10"/>
       <c r="J47" s="10" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="K47" s="9"/>
       <c r="L47" s="9"/>
     </row>
     <row r="48" spans="1:12">
       <c r="A48" s="28" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="C48" s="8" t="s">
         <v>146</v>
@@ -3063,22 +3063,22 @@
       </c>
       <c r="F48" s="10"/>
       <c r="G48" s="10" t="s">
-        <v>169</v>
+        <v>354</v>
       </c>
       <c r="H48" s="10"/>
       <c r="I48" s="10"/>
       <c r="J48" s="10" t="s">
-        <v>170</v>
+        <v>360</v>
       </c>
       <c r="K48" s="9"/>
       <c r="L48" s="9"/>
     </row>
-    <row r="49" spans="1:12" ht="30">
+    <row r="49" spans="1:12">
       <c r="A49" s="28" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>146</v>
@@ -3091,22 +3091,22 @@
       </c>
       <c r="F49" s="10"/>
       <c r="G49" s="10" t="s">
-        <v>171</v>
+        <v>356</v>
       </c>
       <c r="H49" s="10"/>
       <c r="I49" s="10"/>
       <c r="J49" s="10" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="K49" s="9"/>
       <c r="L49" s="9"/>
     </row>
     <row r="50" spans="1:12" ht="45">
       <c r="A50" s="28" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="C50" s="8" t="s">
         <v>146</v>
@@ -3119,24 +3119,24 @@
       </c>
       <c r="F50" s="10"/>
       <c r="G50" s="10" t="s">
-        <v>185</v>
+        <v>357</v>
       </c>
       <c r="H50" s="10"/>
       <c r="I50" s="10"/>
       <c r="J50" s="10" t="s">
-        <v>178</v>
+        <v>361</v>
       </c>
       <c r="K50" s="10" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="L50" s="9"/>
     </row>
-    <row r="51" spans="1:12" ht="60">
+    <row r="51" spans="1:12" ht="45">
       <c r="A51" s="28" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="C51" s="8" t="s">
         <v>146</v>
@@ -3149,24 +3149,24 @@
       </c>
       <c r="F51" s="10"/>
       <c r="G51" s="10" t="s">
-        <v>186</v>
+        <v>358</v>
       </c>
       <c r="H51" s="10"/>
       <c r="I51" s="10"/>
       <c r="J51" s="10" t="s">
-        <v>178</v>
+        <v>361</v>
       </c>
       <c r="K51" s="10" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="L51" s="9"/>
     </row>
     <row r="52" spans="1:12" ht="30">
       <c r="A52" s="9" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="C52" s="8" t="s">
         <v>146</v>
@@ -3179,22 +3179,22 @@
       </c>
       <c r="F52" s="10"/>
       <c r="G52" s="10" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="H52" s="10"/>
       <c r="I52" s="10"/>
       <c r="J52" s="10" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="K52" s="9"/>
       <c r="L52" s="9"/>
     </row>
     <row r="53" spans="1:12">
       <c r="A53" s="9" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>146</v>
@@ -3207,12 +3207,12 @@
       </c>
       <c r="F53" s="10"/>
       <c r="G53" s="10" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="H53" s="10"/>
       <c r="I53" s="10"/>
       <c r="J53" s="10" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="K53" s="9"/>
       <c r="L53" t="s">
@@ -3221,10 +3221,10 @@
     </row>
     <row r="54" spans="1:12" ht="105">
       <c r="A54" s="9" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C54" s="8" t="s">
         <v>146</v>
@@ -3237,15 +3237,15 @@
       </c>
       <c r="F54" s="10"/>
       <c r="G54" s="10" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="H54" s="10"/>
       <c r="I54" s="10"/>
       <c r="J54" s="10" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="K54" s="7" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="L54" t="s">
         <v>116</v>
@@ -3253,31 +3253,31 @@
     </row>
     <row r="55" spans="1:12" ht="60">
       <c r="A55" s="9" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>146</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F55" s="10"/>
       <c r="G55" s="10" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="H55" s="10"/>
       <c r="I55" s="10"/>
       <c r="J55" s="10" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="K55" s="10" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="L55" t="s">
         <v>116</v>
@@ -3285,28 +3285,28 @@
     </row>
     <row r="56" spans="1:12">
       <c r="A56" s="9" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>146</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F56" s="10"/>
       <c r="G56" s="10" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="H56" s="10"/>
       <c r="I56" s="10"/>
       <c r="J56" s="10" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="K56" s="9"/>
       <c r="L56" t="s">
@@ -3315,28 +3315,28 @@
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="9" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>146</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F57" s="10"/>
       <c r="G57" s="10" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="H57" s="10"/>
       <c r="I57" s="10"/>
       <c r="J57" s="10" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="K57" s="9"/>
       <c r="L57" t="s">
@@ -3345,28 +3345,28 @@
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="9" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="C58" s="8" t="s">
         <v>146</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F58" s="10"/>
       <c r="G58" s="10" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="H58" s="10"/>
       <c r="I58" s="10"/>
       <c r="J58" s="10" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="K58" s="9"/>
       <c r="L58" t="s">
@@ -3375,31 +3375,31 @@
     </row>
     <row r="59" spans="1:12" ht="60">
       <c r="A59" s="9" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="C59" s="8" t="s">
         <v>146</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="E59" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F59" s="10"/>
       <c r="G59" s="10" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="H59" s="10"/>
       <c r="I59" s="10"/>
       <c r="J59" s="10" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="K59" s="10" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="L59" t="s">
         <v>116</v>
@@ -3407,31 +3407,31 @@
     </row>
     <row r="60" spans="1:12" ht="30">
       <c r="A60" s="9" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="C60" s="8" t="s">
         <v>146</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F60" s="10"/>
       <c r="G60" s="10" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="H60" s="10"/>
       <c r="I60" s="10"/>
       <c r="J60" s="10" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="K60" s="10" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="L60" t="s">
         <v>116</v>
@@ -3439,31 +3439,31 @@
     </row>
     <row r="61" spans="1:12" ht="30">
       <c r="A61" s="9" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="C61" s="8" t="s">
         <v>146</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F61" s="10"/>
       <c r="G61" s="10" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="H61" s="10"/>
       <c r="I61" s="10"/>
       <c r="J61" s="10" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="K61" s="10" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="L61" t="s">
         <v>116</v>
@@ -3471,31 +3471,31 @@
     </row>
     <row r="62" spans="1:12" ht="30">
       <c r="A62" s="16" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="C62" s="13" t="s">
         <v>146</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="E62" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F62" s="15"/>
       <c r="G62" s="15" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="H62" s="15"/>
       <c r="I62" s="15"/>
       <c r="J62" s="15" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="K62" s="25" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="L62" t="s">
         <v>116</v>
@@ -3503,23 +3503,23 @@
     </row>
     <row r="63" spans="1:12" ht="105">
       <c r="A63" s="24" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="C63" s="8" t="s">
         <v>146</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="E63" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F63" s="10"/>
       <c r="G63" s="10" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="H63" s="10"/>
       <c r="I63" s="10"/>
@@ -3527,7 +3527,7 @@
         <v>27</v>
       </c>
       <c r="K63" s="26" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="L63" t="s">
         <v>116</v>
@@ -3535,23 +3535,23 @@
     </row>
     <row r="64" spans="1:12" ht="30">
       <c r="A64" s="24" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="C64" s="8" t="s">
         <v>146</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="E64" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F64" s="10"/>
       <c r="G64" s="10" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="H64" s="10"/>
       <c r="I64" s="10"/>
@@ -3559,7 +3559,7 @@
         <v>27</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="L64" t="s">
         <v>116</v>
@@ -3567,23 +3567,23 @@
     </row>
     <row r="65" spans="1:12" ht="75">
       <c r="A65" s="24" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="C65" s="8" t="s">
         <v>146</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="E65" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F65" s="10"/>
       <c r="G65" s="10" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="H65" s="10"/>
       <c r="I65" s="10"/>
@@ -3591,7 +3591,7 @@
         <v>27</v>
       </c>
       <c r="K65" s="26" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="L65" t="s">
         <v>116</v>
@@ -3599,28 +3599,28 @@
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="24" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="C66" s="8" t="s">
         <v>146</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F66" s="10"/>
       <c r="G66" s="10" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="H66" s="10"/>
       <c r="I66" s="10"/>
       <c r="J66" s="10" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="K66" s="9"/>
       <c r="L66" t="s">
@@ -3629,23 +3629,23 @@
     </row>
     <row r="67" spans="1:12" ht="30">
       <c r="A67" s="27" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="C67" s="13" t="s">
         <v>146</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="E67" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F67" s="15"/>
       <c r="G67" s="15" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="H67" s="15"/>
       <c r="I67" s="15"/>
@@ -3653,7 +3653,7 @@
         <v>27</v>
       </c>
       <c r="K67" s="15" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="L67" t="s">
         <v>116</v>
@@ -3661,10 +3661,10 @@
     </row>
     <row r="68" spans="1:12" ht="30">
       <c r="A68" s="9" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="C68" s="8" t="s">
         <v>146</v>
@@ -3677,14 +3677,14 @@
       </c>
       <c r="F68" s="10"/>
       <c r="G68" s="10" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="H68" s="10"/>
       <c r="I68" s="10" t="s">
         <v>64</v>
       </c>
       <c r="J68" s="15" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="K68" s="9"/>
       <c r="L68" t="s">
@@ -3693,10 +3693,10 @@
     </row>
     <row r="69" spans="1:12" ht="60">
       <c r="A69" s="16" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="C69" s="13" t="s">
         <v>146</v>
@@ -3709,14 +3709,14 @@
       </c>
       <c r="F69" s="15"/>
       <c r="G69" s="15" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="H69" s="15"/>
       <c r="I69" s="15" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="J69" s="15" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="K69" s="16"/>
       <c r="L69" t="s">
@@ -3725,10 +3725,10 @@
     </row>
     <row r="70" spans="1:12" ht="30">
       <c r="A70" s="9" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="C70" s="8" t="s">
         <v>146</v>
@@ -3741,15 +3741,15 @@
       </c>
       <c r="F70" s="10"/>
       <c r="G70" s="10" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="H70" s="10"/>
       <c r="I70" s="10"/>
       <c r="J70" s="10" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="K70" s="9" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="L70" t="s">
         <v>116</v>
@@ -3757,10 +3757,10 @@
     </row>
     <row r="71" spans="1:12" ht="30">
       <c r="A71" s="9" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="C71" s="8" t="s">
         <v>146</v>
@@ -3773,14 +3773,14 @@
       </c>
       <c r="F71" s="10"/>
       <c r="G71" s="10" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="H71" s="10"/>
       <c r="I71" s="9" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="J71" s="10" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="K71" s="9"/>
       <c r="L71" t="s">
@@ -3789,10 +3789,10 @@
     </row>
     <row r="72" spans="1:12" ht="30">
       <c r="A72" s="9" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="C72" s="8" t="s">
         <v>146</v>
@@ -3805,14 +3805,14 @@
       </c>
       <c r="F72" s="10"/>
       <c r="G72" s="10" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="H72" s="10"/>
       <c r="I72" s="9" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="J72" s="10" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="K72" s="9"/>
       <c r="L72" t="s">
@@ -3821,10 +3821,10 @@
     </row>
     <row r="73" spans="1:12" ht="30">
       <c r="A73" s="9" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="C73" s="8" t="s">
         <v>146</v>
@@ -3837,12 +3837,12 @@
       </c>
       <c r="F73" s="10"/>
       <c r="G73" s="10" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="H73" s="10"/>
       <c r="I73" s="10"/>
       <c r="J73" s="10" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="K73" s="9"/>
       <c r="L73" t="s">
@@ -3851,10 +3851,10 @@
     </row>
     <row r="74" spans="1:12" ht="45">
       <c r="A74" s="16" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="B74" s="15" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="C74" s="13" t="s">
         <v>146</v>
@@ -3867,14 +3867,14 @@
       </c>
       <c r="F74" s="15"/>
       <c r="G74" s="15" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="H74" s="15"/>
       <c r="I74" s="16" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="J74" s="15" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="K74" s="16"/>
       <c r="L74" t="s">
@@ -3883,31 +3883,31 @@
     </row>
     <row r="75" spans="1:12" ht="60">
       <c r="A75" s="16" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="C75" s="8" t="s">
         <v>146</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="E75" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F75" s="10"/>
       <c r="G75" s="10" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="H75" s="10"/>
       <c r="I75" s="10"/>
       <c r="J75" s="10" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="K75" s="10" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="L75" t="s">
         <v>116</v>
@@ -3915,10 +3915,10 @@
     </row>
     <row r="76" spans="1:12" ht="30">
       <c r="A76" s="16" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="B76" s="15" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="C76" s="13" t="s">
         <v>146</v>
@@ -3931,14 +3931,14 @@
       </c>
       <c r="F76" s="15"/>
       <c r="G76" s="15" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="H76" s="15"/>
       <c r="I76" s="1" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="J76" s="10" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="K76" s="9"/>
       <c r="L76" t="s">
@@ -3947,10 +3947,10 @@
     </row>
     <row r="77" spans="1:12" ht="45">
       <c r="A77" s="9" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="B77" s="10" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="C77" s="8" t="s">
         <v>146</v>
@@ -3963,14 +3963,14 @@
       </c>
       <c r="F77" s="10"/>
       <c r="G77" s="10" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="H77" s="10"/>
       <c r="I77" s="10" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="J77" s="10" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="K77" s="9"/>
       <c r="L77" t="s">
@@ -3979,10 +3979,10 @@
     </row>
     <row r="78" spans="1:12" ht="30">
       <c r="A78" s="16" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="C78" s="13" t="s">
         <v>146</v>
@@ -3995,14 +3995,14 @@
       </c>
       <c r="F78" s="15"/>
       <c r="G78" s="15" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="H78" s="15"/>
       <c r="I78" s="1" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="J78" s="15" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="K78" s="16"/>
       <c r="L78" t="s">
@@ -4011,10 +4011,10 @@
     </row>
     <row r="79" spans="1:12" ht="45">
       <c r="A79" s="9" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="C79" s="8" t="s">
         <v>146</v>
@@ -4027,14 +4027,14 @@
       </c>
       <c r="F79" s="10"/>
       <c r="G79" s="10" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="H79" s="10"/>
       <c r="I79" s="10" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="J79" s="10" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="K79" s="9"/>
       <c r="L79" s="9" t="s">
@@ -4043,10 +4043,10 @@
     </row>
     <row r="80" spans="1:12" ht="45">
       <c r="A80" s="9" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="B80" s="10" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="C80" s="8" t="s">
         <v>146</v>
@@ -4059,14 +4059,14 @@
       </c>
       <c r="F80" s="10"/>
       <c r="G80" s="10" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="H80" s="10"/>
       <c r="I80" s="9" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="J80" s="10" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="K80" s="9"/>
       <c r="L80" t="s">
@@ -4075,31 +4075,31 @@
     </row>
     <row r="81" spans="1:12" ht="60">
       <c r="A81" s="16" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="B81" s="15" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="C81" s="13" t="s">
         <v>146</v>
       </c>
       <c r="D81" s="13" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="E81" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F81" s="15"/>
       <c r="G81" s="15" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="H81" s="15"/>
       <c r="I81" s="15"/>
       <c r="J81" s="15" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="K81" s="15" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="L81" t="s">
         <v>116</v>
@@ -4107,257 +4107,256 @@
     </row>
     <row r="82" spans="1:12" ht="105">
       <c r="A82" s="9" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="C82" s="8" t="s">
         <v>146</v>
       </c>
       <c r="D82" s="7" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="E82" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F82" s="10"/>
       <c r="G82" s="10" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="H82" s="10"/>
       <c r="I82" s="24" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="J82" s="10" t="s">
         <v>27</v>
       </c>
       <c r="K82" s="26" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="L82" s="9"/>
     </row>
     <row r="83" spans="1:12" ht="105">
       <c r="A83" s="9" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="C83" s="8" t="s">
         <v>146</v>
       </c>
       <c r="D83" s="7" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="E83" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F83" s="10"/>
       <c r="G83" s="10" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="H83" s="10"/>
       <c r="I83" s="24" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="J83" s="10" t="s">
         <v>27</v>
       </c>
       <c r="K83" s="26" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="L83" s="9"/>
     </row>
     <row r="84" spans="1:12" ht="105">
       <c r="A84" s="9" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="C84" s="8" t="s">
         <v>146</v>
       </c>
       <c r="D84" s="7" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="E84" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F84" s="10"/>
       <c r="G84" s="10" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="H84" s="10"/>
       <c r="I84" s="24" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="J84" s="10" t="s">
         <v>27</v>
       </c>
       <c r="K84" s="26" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="L84" s="9"/>
     </row>
     <row r="85" spans="1:12" ht="105">
       <c r="A85" s="9" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="C85" s="8" t="s">
         <v>146</v>
       </c>
       <c r="D85" s="7" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="E85" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F85" s="10"/>
       <c r="G85" s="10" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="H85" s="10"/>
       <c r="I85" s="24" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="J85" s="10" t="s">
         <v>27</v>
       </c>
       <c r="K85" s="10" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
     </row>
     <row r="86" spans="1:12" ht="105">
       <c r="A86" s="9" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="C86" s="8" t="s">
         <v>146</v>
       </c>
       <c r="D86" s="7" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="E86" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F86" s="10"/>
       <c r="G86" s="10" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="H86" s="10"/>
       <c r="I86" s="24" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="J86" s="10" t="s">
         <v>27</v>
       </c>
       <c r="K86" s="10" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
     </row>
     <row r="87" spans="1:12" ht="105">
       <c r="A87" s="9" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="B87" s="10" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="C87" s="8" t="s">
         <v>146</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="E87" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F87" s="10"/>
       <c r="G87" s="10" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
       <c r="H87" s="10"/>
       <c r="I87" s="24" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="J87" s="10" t="s">
         <v>27</v>
       </c>
       <c r="K87" s="10" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
     </row>
     <row r="88" spans="1:12" ht="105">
       <c r="A88" s="9" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="C88" s="8" t="s">
         <v>146</v>
       </c>
       <c r="D88" s="7" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="E88" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F88" s="10"/>
       <c r="G88" s="10" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="H88" s="10"/>
       <c r="I88" s="24" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="J88" s="10" t="s">
         <v>27</v>
       </c>
       <c r="K88" s="10" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
     </row>
     <row r="89" spans="1:12" ht="105">
       <c r="A89" s="9" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="B89" s="10" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="C89" s="8" t="s">
         <v>146</v>
       </c>
       <c r="D89" s="7" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="E89" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F89" s="10"/>
       <c r="G89" s="10" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="H89" s="10"/>
       <c r="I89" s="24" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="J89" s="10" t="s">
         <v>27</v>
       </c>
       <c r="K89" s="10" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L81"/>
   <hyperlinks>
     <hyperlink ref="A36" r:id="rId1" display="http://ent.jira.int.thomsonreuters.com/browse/WAT-535"/>
   </hyperlinks>

</xml_diff>

<commit_message>
WAT new scripts automation
</commit_message>
<xml_diff>
--- a/src/test/test-data/WATTestData.xlsx
+++ b/src/test/test-data/WATTestData.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="387">
   <si>
     <t>GET</t>
   </si>
@@ -1170,6 +1170,33 @@
   </si>
   <si>
     <t>?name=bhavya&amp;org=indian&amp;fltr=org</t>
+  </si>
+  <si>
+    <t>WAT-1195</t>
+  </si>
+  <si>
+    <t>WAT-1196</t>
+  </si>
+  <si>
+    <t>Verify that ‘Get Author metadata’ also return ‘Total Citing Publications’</t>
+  </si>
+  <si>
+    <t>/author/3515</t>
+  </si>
+  <si>
+    <t>status=200||authorId=3515</t>
+  </si>
+  <si>
+    <t>totalCitingPublications</t>
+  </si>
+  <si>
+    <t>Verify that ‘Get combined Author metadata’ also return ‘Total Citing Publications’</t>
+  </si>
+  <si>
+    <t>?authorId=45&amp;authorId=74</t>
+  </si>
+  <si>
+    <t>status=200||authorIds=45||authorIds=74</t>
   </si>
 </sst>
 </file>
@@ -1680,10 +1707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L93"/>
+  <dimension ref="A1:L95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E41" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J48" sqref="J48"/>
+    <sheetView tabSelected="1" topLeftCell="E88" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K100" sqref="K100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4543,6 +4570,66 @@
       <c r="K93" s="31"/>
       <c r="L93" s="9"/>
     </row>
+    <row r="94" spans="1:12">
+      <c r="A94" s="24" t="s">
+        <v>378</v>
+      </c>
+      <c r="B94" s="10" t="s">
+        <v>380</v>
+      </c>
+      <c r="C94" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D94" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="E94" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F94" s="10"/>
+      <c r="G94" s="9"/>
+      <c r="H94" s="10"/>
+      <c r="I94" s="10"/>
+      <c r="J94" s="10" t="s">
+        <v>382</v>
+      </c>
+      <c r="K94" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="L94" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12">
+      <c r="A95" s="24" t="s">
+        <v>379</v>
+      </c>
+      <c r="B95" s="10" t="s">
+        <v>384</v>
+      </c>
+      <c r="C95" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D95" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="E95" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F95" s="10"/>
+      <c r="G95" s="10" t="s">
+        <v>385</v>
+      </c>
+      <c r="H95" s="10"/>
+      <c r="I95" s="10"/>
+      <c r="J95" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="K95" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="L95" s="9"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A36" r:id="rId1" display="http://ent.jira.int.thomsonreuters.com/browse/WAT-535"/>

</xml_diff>

<commit_message>
WAT new scripts added
</commit_message>
<xml_diff>
--- a/src/test/test-data/WATTestData.xlsx
+++ b/src/test/test-data/WATTestData.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="411">
   <si>
     <t>GET</t>
   </si>
@@ -1222,12 +1222,72 @@
   <si>
     <t>hits[0].authorList||hits[1].authorList||hits[2].authorList||hits[3].authorList||hits[4].authorList||hits[5].authorList||hits[6].authorList||hits[7].authorList||hits[8].authorList||hits[9].authorList</t>
   </si>
+  <si>
+    <t>Verify that Get Recommend Publication API parameters limit and offset default values should be 3 and 0</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Get Recommend Publication API limit parameter should restrict to 10000.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that Get Recommend Publication API should provide recommendations based on set limit and offset. </t>
+  </si>
+  <si>
+    <t>Verify that Get Recommend Publication API limit parameter should override eiddo configuration recommendation.max(3)</t>
+  </si>
+  <si>
+    <t>status=200||offset=0||limit=3</t>
+  </si>
+  <si>
+    <t>?authorId=45&amp;name=wang</t>
+  </si>
+  <si>
+    <t>?authorId=45&amp;name=wang&amp;limit=10</t>
+  </si>
+  <si>
+    <t>status=200||offset=0||limit=10</t>
+  </si>
+  <si>
+    <t>?authorId=45&amp;name=wang&amp;limit=50000</t>
+  </si>
+  <si>
+    <t>status=200||limit=10000</t>
+  </si>
+  <si>
+    <t>?authorId=45&amp;name=wang&amp;limit=10&amp;offset=4</t>
+  </si>
+  <si>
+    <t>status=200||offset=4||limit=10</t>
+  </si>
+  <si>
+    <t>WAT-1325</t>
+  </si>
+  <si>
+    <t>WAT-1322</t>
+  </si>
+  <si>
+    <t>WAT-1323</t>
+  </si>
+  <si>
+    <t>WAT-1324</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1239,6 +1299,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1357,7 +1424,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1436,6 +1503,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1731,16 +1801,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L97"/>
+  <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E89" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L97" sqref="L97"/>
+    <sheetView tabSelected="1" topLeftCell="E90" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="90.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="106.42578125" style="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="80.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
@@ -4714,6 +4784,123 @@
       </c>
       <c r="L97" s="9"/>
     </row>
+    <row r="98" spans="1:12">
+      <c r="A98" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="C98" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D98" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="E98" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F98" s="10"/>
+      <c r="G98" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H98" s="10"/>
+      <c r="I98" s="10"/>
+      <c r="J98" s="10" t="s">
+        <v>399</v>
+      </c>
+      <c r="K98" s="9"/>
+      <c r="L98" s="9"/>
+    </row>
+    <row r="99" spans="1:12" ht="30">
+      <c r="A99" s="9" t="s">
+        <v>409</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="C99" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D99" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="E99" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F99" s="10"/>
+      <c r="G99" s="10" t="s">
+        <v>401</v>
+      </c>
+      <c r="H99" s="10"/>
+      <c r="I99" s="10"/>
+      <c r="J99" s="10" t="s">
+        <v>402</v>
+      </c>
+      <c r="K99" s="9"/>
+      <c r="L99" s="9"/>
+    </row>
+    <row r="100" spans="1:12">
+      <c r="A100" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="C100" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D100" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="E100" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F100" s="10"/>
+      <c r="G100" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H100" s="10"/>
+      <c r="I100" s="10"/>
+      <c r="J100" s="10" t="s">
+        <v>404</v>
+      </c>
+      <c r="K100" s="9"/>
+      <c r="L100" s="9"/>
+    </row>
+    <row r="101" spans="1:12">
+      <c r="A101" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="B101" s="35" t="s">
+        <v>397</v>
+      </c>
+      <c r="C101" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D101" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="E101" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F101" s="10"/>
+      <c r="G101" s="10" t="s">
+        <v>405</v>
+      </c>
+      <c r="H101" s="10"/>
+      <c r="I101" s="10"/>
+      <c r="J101" s="10" t="s">
+        <v>406</v>
+      </c>
+      <c r="K101" s="9"/>
+      <c r="L101" s="9"/>
+    </row>
+    <row r="1048576" spans="4:4">
+      <c r="D1048576" s="7" t="s">
+        <v>232</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A36" r:id="rId1" display="http://ent.jira.int.thomsonreuters.com/browse/WAT-535"/>

</xml_diff>